<commit_message>
modify code and add data
</commit_message>
<xml_diff>
--- a/Second_task/data/address_gps.xlsx
+++ b/Second_task/data/address_gps.xlsx
@@ -18,7 +18,19 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="C55">
+    <comment authorId="0" ref="C12">
+      <text>
+        <t xml:space="preserve">Geocode : 
+Sorry, no results were found for this address. Please retry by reformulating it or looking for wider results.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C186">
+      <text>
+        <t xml:space="preserve">Geocode : 
+Sorry, no results were found for this address. Please retry by reformulating it or looking for wider results.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="C220">
       <text>
         <t xml:space="preserve">Geocode : 
 Sorry, no results were found for this address. Please retry by reformulating it or looking for wider results.</t>
@@ -40,769 +52,769 @@
     <t>Longitude</t>
   </si>
   <si>
+    <t>서울특별시 은평구 수색동 37-36</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 동교동 165</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 공덕동 423-29</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 효창동 80</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 노고산동 31-11</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 용산구 동자동 14-151</t>
+  </si>
+  <si>
+    <t>서울특별시 도봉구 도봉동 38-3</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 월계동 25-2</t>
+  </si>
+  <si>
+    <t>서울특별시 동대문구 전농동 620-69</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 행당동 192</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 옥수동 168-1</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 용산동5가 17-112</t>
+  </si>
+  <si>
+    <t>서울특별시 금천구 가산동 54-3</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 영등포동1가 35</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 신도림동 460-26</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 방이동 89-28</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 석촌동 209</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 잠실동 122</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 반포동 19-11</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 동작동 327-1</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 여의도동 3</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 당산동 6가 323-1</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 양평동2가 33-79</t>
+  </si>
+  <si>
+    <t>서울특별시 중랑구 상봉동 160-7</t>
+  </si>
+  <si>
+    <t>서울특별시 동대문구 신설동 76-5</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 보문동 1가 127-1</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 동선동4가 1</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 방화동 886</t>
+  </si>
+  <si>
+    <t>경기도 성남시 수정구 수진동 4808</t>
+  </si>
+  <si>
+    <t>경기도 성남시 수정구 수진동 2205-1</t>
+  </si>
+  <si>
+    <t>경기도 성남시 수정구 신흥동 2467</t>
+  </si>
+  <si>
+    <t>경기도 성남시 수정구 신흥동 7-4</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 장지동 596-21</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 장지동 201-5</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 문정동 119-4</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 가락동 184-23</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 가락동 459-4</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 잠실동 8</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 잠실동 7-4</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 신천동 19</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 성내동 319</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 천호동 455</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 암사동 501</t>
+  </si>
+  <si>
+    <t>인천광역시 부평구 갈산동 193-45</t>
+  </si>
+  <si>
+    <t>인천광역시 부평구 삼산동 466</t>
+  </si>
+  <si>
+    <t>경기도 부천시 원미구 상동 633</t>
+  </si>
+  <si>
+    <t>경기도 부천시 원미구 중동 1243</t>
+  </si>
+  <si>
+    <t>경기도 부천시 원미구 중동 1140-6</t>
+  </si>
+  <si>
+    <t>경기도 부천시 원미구 춘의동 145</t>
+  </si>
+  <si>
+    <t>경기도 부천시 원미구 춘의동 15-1</t>
+  </si>
+  <si>
+    <t>경기도 부천시 원미구 춘의동 3-1</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 온수동 53-1</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 오류동 174-6</t>
+  </si>
+  <si>
+    <t>경기도 광명시 광명동 158-211</t>
+  </si>
+  <si>
+    <t>경기도 광명시 철산동 526</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 구로동 801-95</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 구로동 1204</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 대림동 1050-17</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 신길동 3599</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 대방동 466-51</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 대방동 406-10</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 상도동 26-20</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 상도1동 702-1</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 상도동 514</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 사당동 산 25-33</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 사당동 144-4</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 방배동 874-16</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 잠원동 103</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 논현동 280</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 논현동 279-67</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 삼성동 111-44</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 청담동 77-76</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 자양동 73-2</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 화양동 7-3</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 화양동 6-3</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 화양동 164-1</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 능동 275-5</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 중곡동 273-2</t>
+  </si>
+  <si>
+    <t>서울특별시 중랑구 면목동 1382-13</t>
+  </si>
+  <si>
+    <t>서울특별시 중랑구 면목동 495</t>
+  </si>
+  <si>
+    <t>서울특별시 중랑구 면목동 282-6</t>
+  </si>
+  <si>
+    <t>서울특별시 중랑구 중화동 50-3</t>
+  </si>
+  <si>
+    <t>서울특별시 중랑구 묵동 189-5</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 공릉동 616-4</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 공릉동 385-4</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 하계동 273-5</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 중계동 503-3</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 상계동 602-5</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 상계동 729-0</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 상계동 650</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 상계동 1132-9</t>
+  </si>
+  <si>
+    <t>경기도 의정부시 장암동 160-8</t>
+  </si>
+  <si>
+    <t>서울특별시 중랑구 신내동 643-1</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 공릉동 285-2</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 석관동 349-8</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 상월곡동 26-1</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 하월곡동 35-1</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 종암동 29-18</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 안암동5가 146-1</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 창신동 20-8</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 숭인동 117</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 창신동 263-2</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 신당동 99</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 흥인동 162-1</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 신당동 295-2</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 신당동 369-44</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 신당동 369-2</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 신당동 366-454</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 한남동 726-494</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 이태원동 119-23</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 용산동 4가 4</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 한강로1가 228-1</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 대흥동 128-1</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 창전동 145-17</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 상수동 309-10</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 서교동 393</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 합정동 414</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 망원동 378</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 성산동 592</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 성산동 420</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 증산동 199-8</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 신사동 337-5</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 구산동 1</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 갈현동 397</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 불광동 13-33</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 대조동 14-1</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 녹번동 144-69</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 역촌동 85-41</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 마천동 307-4</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 거여동 20-14</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 오금동 165-2</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 오금동 44-2</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 방이동 217-2</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 둔촌동 416</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 상일동 148</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 고덕동 310</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 명일동 312</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 명일동 345-12</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 길동 378</t>
+  </si>
+  <si>
+    <t>서울특별시 강동구 천호동 447</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 광장동 237</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 능동 256-16</t>
+  </si>
+  <si>
+    <t>서울특별시 동대문구 장안동 472-3</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 용답동 99</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 마장동 772</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 행당동 317-241</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 금호동2가 223-1</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 을지로 7가 112-3</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 광희동2가 9</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 광희동1가 235-6</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 을지로4가 267-1</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 을지로4가 192</t>
+  </si>
+  <si>
+    <t>서울특별시 종로3가 10-5</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 묘동 59</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 세종로 1-90</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 평동 210</t>
+  </si>
+  <si>
+    <t>서울특별시 서대문구 충정로3가 319-1</t>
+  </si>
+  <si>
+    <t>서울특별시 서대문구 충정로3가 248-1</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 아현동 612</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 도화동 160</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 여의도동 84-4</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 영등포동5가 62-1</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 당산동3가 270-1</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 당산동3가 556-1</t>
+  </si>
+  <si>
+    <t>서울특별시 양천구 목동 406-30</t>
+  </si>
+  <si>
+    <t>서울특별시 양천구 목동 926-3</t>
+  </si>
+  <si>
+    <t>서울특별시 양천구 신정동 1090</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 화곡동 662-5</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 화곡동 1089-54</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 화곡동 1089-3</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 가양동 967-3</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 가양동 530-6</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 공항동 29-5</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 방화동 846</t>
+  </si>
+  <si>
+    <t>서울특별시 강서구 방화동 829-15</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 방배동 2909</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 사당동 1129</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 사당동 588-4</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 사당동 736-1</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 한강로2가 181</t>
+  </si>
+  <si>
+    <t>서울특별시 용산구 갈월동 16-7</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 남창동 64-1</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 충무로2가 109-2</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 필동2가 16-2</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 창신동 492-1</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 종로6가 287-1</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 명륜4가 96-5</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 삼선동1가 14</t>
+  </si>
+  <si>
+    <t>서울특별시 성북구 길음동 877-66</t>
+  </si>
+  <si>
+    <t>서울특별시 강북구 미아동 66-1</t>
+  </si>
+  <si>
+    <t>서울특별시 강북구 미아동 194-1</t>
+  </si>
+  <si>
+    <t>서울특별시 강북구 수유동 140</t>
+  </si>
+  <si>
+    <t>서울특별시 도봉구 창동 703-4</t>
+  </si>
+  <si>
+    <t>서울특별시 도봉구 창동 135-1</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 상계동 156-203</t>
+  </si>
+  <si>
+    <t>서울특별시 노원구 상계동 111</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 가락동 10-15</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 수서동 728</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 일원동 717</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 일원동 700-9</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 대치동 514-3</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 대치동 317-3</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 도곡동 339-2</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 도곡동 179-2</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 서초동 1366-9</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 서초동 1748-30</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 잠원동 100-1</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 신사동 667</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 신사동 668</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 금호동4가 1470</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 장충동2가 199-3</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 을지로3가 347-3</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 을지로3가 282-8</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 안국동 155-2</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 적선동 81-1</t>
+  </si>
+  <si>
+    <t>서울특별시 서대문구 현저동 101</t>
+  </si>
+  <si>
+    <t>서울특별시 서대문구 홍제동 26-1</t>
+  </si>
+  <si>
+    <t>서울특별시 서대문구 홍제동 161-1</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 녹번동 55</t>
+  </si>
+  <si>
+    <t>서울특별시 은평구 진관동 67-26</t>
+  </si>
+  <si>
+    <t>경기도 고양시 덕양구 지축동 818-64</t>
+  </si>
+  <si>
+    <t>서울특별시 동대문구 용두동 47-1</t>
+  </si>
+  <si>
+    <t>서울특별시 양천구 신정동 1231</t>
+  </si>
+  <si>
+    <t>서울특별시 양천구 신정동 276-7</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 신도림동 323-16</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 용답동 129-2</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 용답동 127</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 아현동 354-23</t>
+  </si>
+  <si>
+    <t>서울특별시 마포구 염리동 8-85</t>
+  </si>
+  <si>
+    <t>서울특별시 영등포구 문래동3가 68-1</t>
+  </si>
+  <si>
+    <t>서울특별시 구로구 구로동 810-3</t>
+  </si>
+  <si>
+    <t>서울특별시 동작구 신대방동 643-1</t>
+  </si>
+  <si>
+    <t>서울특별시 관악구 신림동 1467-10</t>
+  </si>
+  <si>
+    <t>서울툭별시 관악구 봉천동 979-7</t>
+  </si>
+  <si>
+    <t>서울특별시 관악구 봉천동 979-2</t>
+  </si>
+  <si>
+    <t>서울특별시 관악구 봉천동 1693-39</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 방배동 912-14</t>
+  </si>
+  <si>
+    <t>서울특별시 서초구 서초동 1748-5</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 역삼동 858</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 역삼동 804</t>
+  </si>
+  <si>
+    <t>서울특별시 강남구 삼성동 172-66</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 잠실동 33</t>
+  </si>
+  <si>
+    <t>서울특별시 송파구 신천동 15</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 구의동 546-6</t>
+  </si>
+  <si>
+    <t>서울특별시 광진구 구의동 245-24</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 성수동2가 300-1</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 성수동1가 656-745</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 행당동 산17 17</t>
+  </si>
+  <si>
+    <t>서울특별시 성동구 하왕십리동 946-14</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 을지로1가 100-1</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 정동 5-5</t>
+  </si>
+  <si>
+    <t>서울특별시 중구 서소문동 90-1</t>
+  </si>
+  <si>
+    <t>서울특별시 동대문구 제기동 65</t>
+  </si>
+  <si>
+    <t>서울특별시 종로구 종로5가 82-1</t>
+  </si>
+  <si>
     <t>서울특별시 종로구 종로1가 54</t>
-  </si>
-  <si>
-    <t>서울특별시 종로3가 10-5</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 묘동 59</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 종로5가 82-1</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 창신동 492-1</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 종로6가 287-1</t>
-  </si>
-  <si>
-    <t>서울특별시 동대문구 신설동 76-5</t>
-  </si>
-  <si>
-    <t>서울특별시 동대문구 제기동 65</t>
-  </si>
-  <si>
-    <t>서울특별시 동대문구 전농동 620-69</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 숭인동 117</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 창신동 263-2</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 정동 5-5</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 서소문동 90-1</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 을지로1가 100-1</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 을지로3가 347-3</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 을지로3가 282-8</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 을지로4가 267-1</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 을지로4가 192</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 을지로 7가 112-3</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 광희동2가 9</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 광희동1가 235-6</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 신당동 99</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 흥인동 162-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 하왕십리동 946-14</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 행당동 192</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 행당동 산17 17</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 성수동1가 656-745</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 성수동2가 300-1</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 화양동 7-3</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 화양동 6-3</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 구의동 245-24</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 구의동 546-6</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 신천동 15</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 잠실동 8</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 잠실동 7-4</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 잠실동 33</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 잠실동 122</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 삼성동 172-66</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 역삼동 804</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 역삼동 858</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 서초동 1748-5</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 방배동 912-14</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 사당동 1129</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 사당동 588-4</t>
-  </si>
-  <si>
-    <t>서울특별시 관악구 봉천동 1693-39</t>
-  </si>
-  <si>
-    <t>서울특별시 관악구 봉천동 979-2</t>
-  </si>
-  <si>
-    <t>서울툭별시 관악구 봉천동 979-7</t>
-  </si>
-  <si>
-    <t>서울특별시 관악구 신림동 1467-10</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 신대방동 643-1</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 구로동 810-3</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 구로동 1204</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 대림동 1050-17</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 신도림동 460-26</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 문래동3가 68-1</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 당산동3가 270-1</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 당산동3가 556-1</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 당산동 6가 323-1</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 서교동 393</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 합정동 414</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 동교동 165</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 노고산동 31-11</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 염리동 8-85</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 아현동 354-23</t>
-  </si>
-  <si>
-    <t>서울특별시 서대문구 충정로3가 319-1</t>
-  </si>
-  <si>
-    <t>서울특별시 서대문구 충정로3가 248-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 용답동 127</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 용답동 129-2</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 신도림동 323-16</t>
-  </si>
-  <si>
-    <t>서울특별시 양천구 신정동 276-7</t>
-  </si>
-  <si>
-    <t>서울특별시 양천구 신정동 1231</t>
-  </si>
-  <si>
-    <t>서울특별시 동대문구 용두동 47-1</t>
-  </si>
-  <si>
-    <t>경기도 고양시 덕양구 지축동 818-64</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 진관동 67-26</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 갈현동 397</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 대조동 14-1</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 녹번동 55</t>
-  </si>
-  <si>
-    <t>서울특별시 서대문구 홍제동 161-1</t>
-  </si>
-  <si>
-    <t>서울특별시 서대문구 홍제동 26-1</t>
-  </si>
-  <si>
-    <t>서울특별시 서대문구 현저동 101</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 적선동 81-1</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 안국동 155-2</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 필동2가 16-2</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 장충동2가 199-3</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 신당동 369-44</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 신당동 369-2</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 금호동4가 1470</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 옥수동 168-1</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 신사동 668</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 신사동 667</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 잠원동 100-1</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 반포동 19-11</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 서초동 1748-30</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 서초동 1366-9</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 도곡동 179-2</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 도곡동 339-2</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 대치동 317-3</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 대치동 514-3</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 일원동 700-9</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 일원동 717</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 수서동 728</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 가락동 184-23</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 가락동 10-15</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 오금동 44-2</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 상계동 111</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 상계동 156-203</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 상계동 602-5</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 상계동 729-0</t>
-  </si>
-  <si>
-    <t>서울특별시 도봉구 창동 135-1</t>
-  </si>
-  <si>
-    <t>서울특별시 도봉구 창동 703-4</t>
-  </si>
-  <si>
-    <t>서울특별시 강북구 수유동 140</t>
-  </si>
-  <si>
-    <t>서울특별시 강북구 미아동 194-1</t>
-  </si>
-  <si>
-    <t>서울특별시 강북구 미아동 66-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 길음동 877-66</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 동선동4가 1</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 삼선동1가 14</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 명륜4가 96-5</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 충무로2가 109-2</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 남창동 64-1</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 용산구 동자동 14-151</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 갈월동 16-7</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 한강로1가 228-1</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 한강로2가 181</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 용산동5가 17-112</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 동작동 327-1</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 사당동 736-1</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 방배동 2909</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 영등포동1가 35</t>
-  </si>
-  <si>
-    <t>서울특별시 금천구 가산동 54-3</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 온수동 53-1</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 월계동 25-2</t>
-  </si>
-  <si>
-    <t>서울특별시 도봉구 도봉동 38-3</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 삼성동 111-44</t>
-  </si>
-  <si>
-    <t>경기도 성남시 수정구 수진동 4808</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구 상봉동 160-7</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 양평동2가 33-79</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 효창동 80</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 공덕동 423-29</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 수색동 37-36</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 방화동 829-15</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 방화동 846</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 방화동 886</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 공항동 29-5</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 가양동 530-6</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 가양동 967-3</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 화곡동 1089-3</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 화곡동 1089-54</t>
-  </si>
-  <si>
-    <t>서울특별시 강서구 화곡동 662-5</t>
-  </si>
-  <si>
-    <t>서울특별시 양천구 신정동 1090</t>
-  </si>
-  <si>
-    <t>서울특별시 양천구 목동 926-3</t>
-  </si>
-  <si>
-    <t>서울특별시 양천구 목동 406-30</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 영등포동5가 62-1</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 여의도동 3</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 여의도동 84-4</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 도화동 160</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 아현동 612</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 평동 210</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 세종로 1-90</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 신당동 295-2</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 금호동2가 223-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 행당동 317-241</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 마장동 772</t>
-  </si>
-  <si>
-    <t>서울특별시 성동구 용답동 99</t>
-  </si>
-  <si>
-    <t>서울특별시 동대문구 장안동 472-3</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 능동 275-5</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 능동 256-16</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 광장동 237</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 천호동 455</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 천호동 447</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 길동 378</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 명일동 345-12</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 명일동 312</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 고덕동 310</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 상일동 148</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 둔촌동 416</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 방이동 89-28</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 방이동 217-2</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 오금동 165-2</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 거여동 20-14</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 마천동 307-4</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 역촌동 85-41</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 녹번동 144-69</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 불광동 13-33</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 구산동 1</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 신사동 337-5</t>
-  </si>
-  <si>
-    <t>서울특별시 은평구 증산동 199-8</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 성산동 420</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 성산동 592</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 망원동 378</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 상수동 309-10</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 창전동 145-17</t>
-  </si>
-  <si>
-    <t>서울특별시 마포구 대흥동 128-1</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 용산동 4가 4</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 이태원동 119-23</t>
-  </si>
-  <si>
-    <t>서울특별시 용산구 한남동 726-494</t>
-  </si>
-  <si>
-    <t>서울특별시 중구 신당동 366-454</t>
-  </si>
-  <si>
-    <t>서울특별시 종로구 창신동 20-8</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 보문동 1가 127-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 안암동5가 146-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 종암동 29-18</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 하월곡동 35-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 상월곡동 26-1</t>
-  </si>
-  <si>
-    <t>서울특별시 성북구 석관동 349-8</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 공릉동 616-4</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 공릉동 285-2</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구 신내동 643-1</t>
-  </si>
-  <si>
-    <t>경기도 의정부시 장암동 160-8</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 상계동 1132-9</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 상계동 650</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 중계동 503-3</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 하계동 273-5</t>
-  </si>
-  <si>
-    <t>서울특별시 노원구 공릉동 385-4</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구 묵동 189-5</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구 중화동 50-3</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구 면목동 282-6</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구 면목동 495</t>
-  </si>
-  <si>
-    <t>서울특별시 중랑구 면목동 1382-13</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 중곡동 273-2</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 화양동 164-1</t>
-  </si>
-  <si>
-    <t>서울특별시 광진구 자양동 73-2</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 청담동 77-76</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 논현동 279-67</t>
-  </si>
-  <si>
-    <t>서울특별시 강남구 논현동 280</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 잠원동 103</t>
-  </si>
-  <si>
-    <t>서울특별시 서초구 방배동 874-16</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 사당동 144-4</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 사당동 산 25-33</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 상도동 514</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 상도1동 702-1</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 상도동 26-20</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 대방동 406-10</t>
-  </si>
-  <si>
-    <t>서울특별시 동작구 대방동 466-51</t>
-  </si>
-  <si>
-    <t>서울특별시 영등포구 신길동 3599</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 구로동 801-95</t>
-  </si>
-  <si>
-    <t>경기도 광명시 철산동 526</t>
-  </si>
-  <si>
-    <t>경기도 광명시 광명동 158-211</t>
-  </si>
-  <si>
-    <t>서울특별시 구로구 오류동 174-6</t>
-  </si>
-  <si>
-    <t>경기도 부천시 원미구 춘의동 3-1</t>
-  </si>
-  <si>
-    <t>경기도 부천시 원미구 춘의동 15-1</t>
-  </si>
-  <si>
-    <t>경기도 부천시 원미구 춘의동 145</t>
-  </si>
-  <si>
-    <t>경기도 부천시 원미구 중동 1140-6</t>
-  </si>
-  <si>
-    <t>경기도 부천시 원미구 중동 1243</t>
-  </si>
-  <si>
-    <t>경기도 부천시 원미구 상동 633</t>
-  </si>
-  <si>
-    <t>인천광역시 부평구 삼산동 466</t>
-  </si>
-  <si>
-    <t>인천광역시 부평구 갈산동 193-45</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 암사동 501</t>
-  </si>
-  <si>
-    <t>서울특별시 강동구 성내동 319</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 신천동 19</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 석촌동 209</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 가락동 459-4</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 문정동 119-4</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 장지동 201-5</t>
-  </si>
-  <si>
-    <t>서울특별시 송파구 장지동 596-21</t>
-  </si>
-  <si>
-    <t>경기도 성남시 수정구 신흥동 7-4</t>
-  </si>
-  <si>
-    <t>경기도 성남시 수정구 신흥동 2467</t>
-  </si>
-  <si>
-    <t>경기도 성남시 수정구 수진동 2205-1</t>
   </si>
 </sst>
 </file>
@@ -826,8 +838,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -888,10 +900,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>37.5701747</v>
+        <v>37.5768989</v>
       </c>
       <c r="C2" s="1">
-        <v>126.9832262</v>
+        <v>126.9016424</v>
       </c>
     </row>
     <row r="3">
@@ -899,10 +911,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>37.5703842</v>
+        <v>37.5567292</v>
       </c>
       <c r="C3" s="1">
-        <v>126.9920077</v>
+        <v>126.9236419</v>
       </c>
     </row>
     <row r="4">
@@ -910,10 +922,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>37.5711966</v>
+        <v>37.5444535</v>
       </c>
       <c r="C4" s="1">
-        <v>126.9919594</v>
+        <v>126.9511752</v>
       </c>
     </row>
     <row r="5">
@@ -921,10 +933,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>37.5708657</v>
+        <v>37.5394453</v>
       </c>
       <c r="C5" s="1">
-        <v>127.0019064</v>
+        <v>126.9611372</v>
       </c>
     </row>
     <row r="6">
@@ -932,10 +944,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>37.5717429</v>
+        <v>37.5546671</v>
       </c>
       <c r="C6" s="1">
-        <v>127.0111694</v>
+        <v>126.9374995</v>
       </c>
     </row>
     <row r="7">
@@ -943,10 +955,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>37.5703848</v>
+        <v>37.5530656</v>
       </c>
       <c r="C7" s="1">
-        <v>127.009529</v>
+        <v>126.9727965</v>
       </c>
     </row>
     <row r="8">
@@ -954,10 +966,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>37.5760874</v>
+        <v>37.6890803</v>
       </c>
       <c r="C8" s="1">
-        <v>127.0245602</v>
+        <v>127.046509</v>
       </c>
     </row>
     <row r="9">
@@ -965,10 +977,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>37.5781628</v>
+        <v>37.6152323</v>
       </c>
       <c r="C9" s="1">
-        <v>127.0346872</v>
+        <v>127.066831</v>
       </c>
     </row>
     <row r="10">
@@ -987,21 +999,21 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>37.5732808</v>
+        <v>37.5622586</v>
       </c>
       <c r="C11" s="1">
-        <v>127.0166486</v>
+        <v>127.0372276</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
-        <v>37.5729495</v>
-      </c>
-      <c r="C12" s="1">
-        <v>127.0156058</v>
+      <c r="B12" s="2">
+        <v>37.539904</v>
+      </c>
+      <c r="C12" s="2">
+        <v>127.017218</v>
       </c>
     </row>
     <row r="13">
@@ -1009,10 +1021,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>37.565682</v>
+        <v>37.5224811</v>
       </c>
       <c r="C13" s="1">
-        <v>126.9768488</v>
+        <v>126.9736707</v>
       </c>
     </row>
     <row r="14">
@@ -1020,10 +1032,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>37.5635313</v>
+        <v>37.4809056</v>
       </c>
       <c r="C14" s="1">
-        <v>126.9755029</v>
+        <v>126.8828399</v>
       </c>
     </row>
     <row r="15">
@@ -1031,10 +1043,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>37.5660664</v>
+        <v>37.5176664</v>
       </c>
       <c r="C15" s="1">
-        <v>126.9820222</v>
+        <v>126.9146626</v>
       </c>
     </row>
     <row r="16">
@@ -1042,10 +1054,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>37.56617</v>
+        <v>37.5086867</v>
       </c>
       <c r="C16" s="1">
-        <v>126.9902025</v>
+        <v>126.8909033</v>
       </c>
     </row>
     <row r="17">
@@ -1053,10 +1065,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="1">
-        <v>37.5664121</v>
+        <v>37.5164494</v>
       </c>
       <c r="C17" s="1">
-        <v>126.9941848</v>
+        <v>127.1311068</v>
       </c>
     </row>
     <row r="18">
@@ -1064,10 +1076,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>37.5664887999999</v>
+        <v>37.5067662</v>
       </c>
       <c r="C18" s="1">
-        <v>126.996528</v>
+        <v>127.1054591</v>
       </c>
     </row>
     <row r="19">
@@ -1075,10 +1087,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>37.5661417</v>
+        <v>37.5110736</v>
       </c>
       <c r="C19" s="1">
-        <v>126.9985136</v>
+        <v>127.0742826</v>
       </c>
     </row>
     <row r="20">
@@ -1086,10 +1098,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>37.5657177</v>
+        <v>37.5047736</v>
       </c>
       <c r="C20" s="1">
-        <v>127.0084849</v>
+        <v>127.0049178</v>
       </c>
     </row>
     <row r="21">
@@ -1097,10 +1109,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>37.5644784</v>
+        <v>37.5034646999999</v>
       </c>
       <c r="C21" s="1">
-        <v>127.0071588</v>
+        <v>126.9799265</v>
       </c>
     </row>
     <row r="22">
@@ -1108,10 +1120,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>37.5645651</v>
+        <v>37.5235124</v>
       </c>
       <c r="C22" s="1">
-        <v>127.0062216</v>
+        <v>126.9264939</v>
       </c>
     </row>
     <row r="23">
@@ -1119,10 +1131,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>37.5652813</v>
+        <v>37.5349309</v>
       </c>
       <c r="C23" s="1">
-        <v>127.0166395</v>
+        <v>126.9027301</v>
       </c>
     </row>
     <row r="24">
@@ -1130,10 +1142,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>37.567534</v>
+        <v>37.5251429</v>
       </c>
       <c r="C24" s="1">
-        <v>127.0161118</v>
+        <v>126.8860734</v>
       </c>
     </row>
     <row r="25">
@@ -1141,10 +1153,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>37.5639331</v>
+        <v>37.5959947</v>
       </c>
       <c r="C25" s="1">
-        <v>127.0297931</v>
+        <v>127.0843699</v>
       </c>
     </row>
     <row r="26">
@@ -1152,10 +1164,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="1">
-        <v>37.5622586</v>
+        <v>37.5760874</v>
       </c>
       <c r="C26" s="1">
-        <v>127.0372276</v>
+        <v>127.0245602</v>
       </c>
     </row>
     <row r="27">
@@ -1163,10 +1175,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="1">
-        <v>37.5552593</v>
+        <v>37.5855633</v>
       </c>
       <c r="C27" s="1">
-        <v>127.0436579</v>
+        <v>127.0201782</v>
       </c>
     </row>
     <row r="28">
@@ -1174,10 +1186,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>37.5471773</v>
+        <v>37.5930482</v>
       </c>
       <c r="C28" s="1">
-        <v>127.0473802</v>
+        <v>127.0167136</v>
       </c>
     </row>
     <row r="29">
@@ -1185,10 +1197,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="1">
-        <v>37.5446009</v>
+        <v>37.5667733</v>
       </c>
       <c r="C29" s="1">
-        <v>127.0568847</v>
+        <v>126.8025118</v>
       </c>
     </row>
     <row r="30">
@@ -1196,10 +1208,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>37.5407487</v>
+        <v>37.4398574</v>
       </c>
       <c r="C30" s="1">
-        <v>127.0690014</v>
+        <v>127.1276594</v>
       </c>
     </row>
     <row r="31">
@@ -1207,10 +1219,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="1">
-        <v>37.5405169</v>
+        <v>37.4374237</v>
       </c>
       <c r="C31" s="1">
-        <v>127.0690846</v>
+        <v>127.1403404</v>
       </c>
     </row>
     <row r="32">
@@ -1218,10 +1230,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="1">
-        <v>37.5382826</v>
+        <v>37.4407489</v>
       </c>
       <c r="C32" s="1">
-        <v>127.0907553</v>
+        <v>127.1463494</v>
       </c>
     </row>
     <row r="33">
@@ -1229,10 +1241,10 @@
         <v>34</v>
       </c>
       <c r="B33" s="1">
-        <v>37.5354211</v>
+        <v>37.4564664</v>
       </c>
       <c r="C33" s="1">
-        <v>127.094533</v>
+        <v>127.1500093</v>
       </c>
     </row>
     <row r="34">
@@ -1240,10 +1252,10 @@
         <v>35</v>
       </c>
       <c r="B34" s="1">
-        <v>37.5186216</v>
+        <v>37.4706864</v>
       </c>
       <c r="C34" s="1">
-        <v>127.1049002</v>
+        <v>127.1266998</v>
       </c>
     </row>
     <row r="35">
@@ -1251,10 +1263,10 @@
         <v>36</v>
       </c>
       <c r="B35" s="1">
-        <v>37.5176605</v>
+        <v>37.4776196</v>
       </c>
       <c r="C35" s="1">
-        <v>127.0746594</v>
+        <v>127.1265061</v>
       </c>
     </row>
     <row r="36">
@@ -1262,10 +1274,10 @@
         <v>37</v>
       </c>
       <c r="B36" s="1">
-        <v>37.5175738</v>
+        <v>37.4881176</v>
       </c>
       <c r="C36" s="1">
-        <v>127.0701491</v>
+        <v>127.1211404</v>
       </c>
     </row>
     <row r="37">
@@ -1273,10 +1285,10 @@
         <v>38</v>
       </c>
       <c r="B37" s="1">
-        <v>37.5115681</v>
+        <v>37.4928982</v>
       </c>
       <c r="C37" s="1">
-        <v>127.0906077</v>
+        <v>127.1180582</v>
       </c>
     </row>
     <row r="38">
@@ -1284,10 +1296,10 @@
         <v>39</v>
       </c>
       <c r="B38" s="1">
-        <v>37.5110736</v>
+        <v>37.4997126</v>
       </c>
       <c r="C38" s="1">
-        <v>127.0742826</v>
+        <v>127.1122396</v>
       </c>
     </row>
     <row r="39">
@@ -1295,10 +1307,10 @@
         <v>40</v>
       </c>
       <c r="B39" s="1">
-        <v>37.5088263</v>
+        <v>37.5176605</v>
       </c>
       <c r="C39" s="1">
-        <v>127.0630673</v>
+        <v>127.0746594</v>
       </c>
     </row>
     <row r="40">
@@ -1306,10 +1318,10 @@
         <v>41</v>
       </c>
       <c r="B40" s="1">
-        <v>37.4981284</v>
+        <v>37.5175738</v>
       </c>
       <c r="C40" s="1">
-        <v>127.028303</v>
+        <v>127.0701491</v>
       </c>
     </row>
     <row r="41">
@@ -1317,10 +1329,10 @@
         <v>42</v>
       </c>
       <c r="B41" s="1">
-        <v>37.4970171999999</v>
+        <v>37.5169204</v>
       </c>
       <c r="C41" s="1">
-        <v>127.0281681</v>
+        <v>127.1107338</v>
       </c>
     </row>
     <row r="42">
@@ -1328,10 +1340,10 @@
         <v>43</v>
       </c>
       <c r="B42" s="1">
-        <v>37.4927648</v>
+        <v>37.5304447</v>
       </c>
       <c r="C42" s="1">
-        <v>127.0105414</v>
+        <v>127.1205399</v>
       </c>
     </row>
     <row r="43">
@@ -1339,10 +1351,10 @@
         <v>44</v>
       </c>
       <c r="B43" s="1">
-        <v>37.4812965</v>
+        <v>37.5384618</v>
       </c>
       <c r="C43" s="1">
-        <v>126.9973202</v>
+        <v>127.1250941</v>
       </c>
     </row>
     <row r="44">
@@ -1350,10 +1362,10 @@
         <v>45</v>
       </c>
       <c r="B44" s="1">
-        <v>37.4764838</v>
+        <v>37.5511434999999</v>
       </c>
       <c r="C44" s="1">
-        <v>126.9813957</v>
+        <v>127.1281759</v>
       </c>
     </row>
     <row r="45">
@@ -1361,10 +1373,10 @@
         <v>46</v>
       </c>
       <c r="B45" s="1">
-        <v>37.4771295</v>
+        <v>37.5075879</v>
       </c>
       <c r="C45" s="1">
-        <v>126.9816651</v>
+        <v>126.7208921</v>
       </c>
     </row>
     <row r="46">
@@ -1372,10 +1384,10 @@
         <v>47</v>
       </c>
       <c r="B46" s="1">
-        <v>37.4770283</v>
+        <v>37.5068138</v>
       </c>
       <c r="C46" s="1">
-        <v>126.9633959</v>
+        <v>126.7368787</v>
       </c>
     </row>
     <row r="47">
@@ -1383,10 +1395,10 @@
         <v>48</v>
       </c>
       <c r="B47" s="1">
-        <v>37.4811133</v>
+        <v>37.5058397</v>
       </c>
       <c r="C47" s="1">
-        <v>126.9526344</v>
+        <v>126.7530584</v>
       </c>
     </row>
     <row r="48">
@@ -1394,10 +1406,10 @@
         <v>49</v>
       </c>
       <c r="B48" s="1">
-        <v>37.4825178</v>
+        <v>37.504159</v>
       </c>
       <c r="C48" s="1">
-        <v>126.941481</v>
+        <v>126.7672837</v>
       </c>
     </row>
     <row r="49">
@@ -1405,10 +1417,10 @@
         <v>50</v>
       </c>
       <c r="B49" s="1">
-        <v>37.4897586</v>
+        <v>37.501902</v>
       </c>
       <c r="C49" s="1">
-        <v>126.9230375</v>
+        <v>126.7762146</v>
       </c>
     </row>
     <row r="50">
@@ -1416,10 +1428,10 @@
         <v>51</v>
       </c>
       <c r="B50" s="1">
-        <v>37.4875104</v>
+        <v>37.5038999</v>
       </c>
       <c r="C50" s="1">
-        <v>126.9129914</v>
+        <v>126.7887438</v>
       </c>
     </row>
     <row r="51">
@@ -1427,10 +1439,10 @@
         <v>52</v>
       </c>
       <c r="B51" s="1">
-        <v>37.4851265</v>
+        <v>37.5050427</v>
       </c>
       <c r="C51" s="1">
-        <v>126.9015288</v>
+        <v>126.7960011</v>
       </c>
     </row>
     <row r="52">
@@ -1438,10 +1450,10 @@
         <v>53</v>
       </c>
       <c r="B52" s="1">
-        <v>37.4925043</v>
+        <v>37.5060988</v>
       </c>
       <c r="C52" s="1">
-        <v>126.8949615</v>
+        <v>126.8011495</v>
       </c>
     </row>
     <row r="53">
@@ -1449,10 +1461,10 @@
         <v>54</v>
       </c>
       <c r="B53" s="1">
-        <v>37.4927052</v>
+        <v>37.4922113</v>
       </c>
       <c r="C53" s="1">
-        <v>126.8966027</v>
+        <v>126.823298</v>
       </c>
     </row>
     <row r="54">
@@ -1460,21 +1472,21 @@
         <v>55</v>
       </c>
       <c r="B54" s="1">
-        <v>37.5086867</v>
+        <v>37.4868662</v>
       </c>
       <c r="C54" s="1">
-        <v>126.8909033</v>
+        <v>126.8388469</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="2">
-        <v>37.517892</v>
-      </c>
-      <c r="C55" s="2">
-        <v>126.894751</v>
+      <c r="B55" s="1">
+        <v>37.4792784</v>
+      </c>
+      <c r="C55" s="1">
+        <v>126.8547139</v>
       </c>
     </row>
     <row r="56">
@@ -1482,10 +1494,10 @@
         <v>57</v>
       </c>
       <c r="B56" s="1">
-        <v>37.5256563</v>
+        <v>37.4760554</v>
       </c>
       <c r="C56" s="1">
-        <v>126.8966142</v>
+        <v>126.8679003</v>
       </c>
     </row>
     <row r="57">
@@ -1493,10 +1505,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="1">
-        <v>37.5243614</v>
+        <v>37.4860727</v>
       </c>
       <c r="C57" s="1">
-        <v>126.894287</v>
+        <v>126.8872892</v>
       </c>
     </row>
     <row r="58">
@@ -1504,10 +1516,10 @@
         <v>59</v>
       </c>
       <c r="B58" s="1">
-        <v>37.5349309</v>
+        <v>37.4925043</v>
       </c>
       <c r="C58" s="1">
-        <v>126.9027301</v>
+        <v>126.8949615</v>
       </c>
     </row>
     <row r="59">
@@ -1515,10 +1527,10 @@
         <v>60</v>
       </c>
       <c r="B59" s="1">
-        <v>37.5500076999999</v>
+        <v>37.4927052</v>
       </c>
       <c r="C59" s="1">
-        <v>126.9145039</v>
+        <v>126.8966027</v>
       </c>
     </row>
     <row r="60">
@@ -1526,10 +1538,10 @@
         <v>61</v>
       </c>
       <c r="B60" s="1">
-        <v>37.5489656</v>
+        <v>37.5002786</v>
       </c>
       <c r="C60" s="1">
-        <v>126.9134767</v>
+        <v>126.9094236</v>
       </c>
     </row>
     <row r="61">
@@ -1537,10 +1549,10 @@
         <v>62</v>
       </c>
       <c r="B61" s="1">
-        <v>37.5567292</v>
+        <v>37.4998736999999</v>
       </c>
       <c r="C61" s="1">
-        <v>126.9236419</v>
+        <v>126.9205715</v>
       </c>
     </row>
     <row r="62">
@@ -1548,10 +1560,10 @@
         <v>63</v>
       </c>
       <c r="B62" s="1">
-        <v>37.5546671</v>
+        <v>37.4996863</v>
       </c>
       <c r="C62" s="1">
-        <v>126.9374995</v>
+        <v>126.9280893</v>
       </c>
     </row>
     <row r="63">
@@ -1559,10 +1571,10 @@
         <v>64</v>
       </c>
       <c r="B63" s="1">
-        <v>37.5568129</v>
+        <v>37.5045422</v>
       </c>
       <c r="C63" s="1">
-        <v>126.9477118</v>
+        <v>126.9385948</v>
       </c>
     </row>
     <row r="64">
@@ -1570,10 +1582,10 @@
         <v>65</v>
       </c>
       <c r="B64" s="1">
-        <v>37.5558896</v>
+        <v>37.5028025</v>
       </c>
       <c r="C64" s="1">
-        <v>126.9556609</v>
+        <v>126.9476764</v>
       </c>
     </row>
     <row r="65">
@@ -1581,10 +1593,10 @@
         <v>66</v>
       </c>
       <c r="B65" s="1">
-        <v>37.5594926</v>
+        <v>37.4957957</v>
       </c>
       <c r="C65" s="1">
-        <v>126.9638176</v>
+        <v>126.9540341</v>
       </c>
     </row>
     <row r="66">
@@ -1592,10 +1604,10 @@
         <v>67</v>
       </c>
       <c r="B66" s="1">
-        <v>37.5611255</v>
+        <v>37.4844029</v>
       </c>
       <c r="C66" s="1">
-        <v>126.9635279</v>
+        <v>126.9716975</v>
       </c>
     </row>
     <row r="67">
@@ -1603,10 +1615,10 @@
         <v>68</v>
       </c>
       <c r="B67" s="1">
-        <v>37.5586888</v>
+        <v>37.4849508</v>
       </c>
       <c r="C67" s="1">
-        <v>127.0531724</v>
+        <v>126.980963</v>
       </c>
     </row>
     <row r="68">
@@ -1614,10 +1626,10 @@
         <v>69</v>
       </c>
       <c r="B68" s="1">
-        <v>37.569744</v>
+        <v>37.4882577</v>
       </c>
       <c r="C68" s="1">
-        <v>127.0469446</v>
+        <v>126.9931587</v>
       </c>
     </row>
     <row r="69">
@@ -1625,10 +1637,10 @@
         <v>70</v>
       </c>
       <c r="B69" s="1">
-        <v>37.5144011</v>
+        <v>37.508249</v>
       </c>
       <c r="C69" s="1">
-        <v>126.8826846</v>
+        <v>127.0118029</v>
       </c>
     </row>
     <row r="70">
@@ -1636,10 +1648,10 @@
         <v>71</v>
       </c>
       <c r="B70" s="1">
-        <v>37.5125175</v>
+        <v>37.5103093</v>
       </c>
       <c r="C70" s="1">
-        <v>126.8657108</v>
+        <v>127.0218222</v>
       </c>
     </row>
     <row r="71">
@@ -1647,10 +1659,10 @@
         <v>72</v>
       </c>
       <c r="B71" s="1">
-        <v>37.5182935</v>
+        <v>37.5111584</v>
       </c>
       <c r="C71" s="1">
-        <v>126.8536189</v>
+        <v>127.0216392</v>
       </c>
     </row>
     <row r="72">
@@ -1658,10 +1670,10 @@
         <v>73</v>
       </c>
       <c r="B72" s="1">
-        <v>37.5738576</v>
+        <v>37.517161</v>
       </c>
       <c r="C72" s="1">
-        <v>127.0379896</v>
+        <v>127.041288</v>
       </c>
     </row>
     <row r="73">
@@ -1669,10 +1681,10 @@
         <v>74</v>
       </c>
       <c r="B73" s="1">
-        <v>37.6487977</v>
+        <v>37.5191066</v>
       </c>
       <c r="C73" s="1">
-        <v>126.9108511</v>
+        <v>127.0520336</v>
       </c>
     </row>
     <row r="74">
@@ -1680,10 +1692,10 @@
         <v>75</v>
       </c>
       <c r="B74" s="1">
-        <v>37.6375367</v>
+        <v>37.5319161</v>
       </c>
       <c r="C74" s="1">
-        <v>126.9185875</v>
+        <v>127.0669943</v>
       </c>
     </row>
     <row r="75">
@@ -1691,10 +1703,10 @@
         <v>76</v>
       </c>
       <c r="B75" s="1">
-        <v>37.6188881</v>
+        <v>37.5407487</v>
       </c>
       <c r="C75" s="1">
-        <v>126.920832</v>
+        <v>127.0690014</v>
       </c>
     </row>
     <row r="76">
@@ -1702,10 +1714,10 @@
         <v>77</v>
       </c>
       <c r="B76" s="1">
-        <v>37.6104829</v>
+        <v>37.5405169</v>
       </c>
       <c r="C76" s="1">
-        <v>126.9292884</v>
+        <v>127.0690846</v>
       </c>
     </row>
     <row r="77">
@@ -1713,10 +1725,10 @@
         <v>78</v>
       </c>
       <c r="B77" s="1">
-        <v>37.6007016999999</v>
+        <v>37.5471128999999</v>
       </c>
       <c r="C77" s="1">
-        <v>126.9360048</v>
+        <v>127.0739401</v>
       </c>
     </row>
     <row r="78">
@@ -1724,10 +1736,10 @@
         <v>79</v>
       </c>
       <c r="B78" s="1">
-        <v>37.5872664</v>
+        <v>37.5569984</v>
       </c>
       <c r="C78" s="1">
-        <v>126.9458373</v>
+        <v>127.079719</v>
       </c>
     </row>
     <row r="79">
@@ -1735,10 +1747,10 @@
         <v>80</v>
       </c>
       <c r="B79" s="1">
-        <v>37.5823607</v>
+        <v>37.5657147</v>
       </c>
       <c r="C79" s="1">
-        <v>126.9504375</v>
+        <v>127.0841917</v>
       </c>
     </row>
     <row r="80">
@@ -1746,10 +1758,10 @@
         <v>81</v>
       </c>
       <c r="B80" s="1">
-        <v>37.5743009</v>
+        <v>37.5734436</v>
       </c>
       <c r="C80" s="1">
-        <v>126.9559178</v>
+        <v>127.0864823</v>
       </c>
     </row>
     <row r="81">
@@ -1757,10 +1769,10 @@
         <v>82</v>
       </c>
       <c r="B81" s="1">
-        <v>37.5758199</v>
+        <v>37.5817877</v>
       </c>
       <c r="C81" s="1">
-        <v>126.9730579</v>
+        <v>127.0843345</v>
       </c>
     </row>
     <row r="82">
@@ -1768,10 +1780,10 @@
         <v>83</v>
       </c>
       <c r="B82" s="1">
-        <v>37.576696</v>
+        <v>37.5891527</v>
       </c>
       <c r="C82" s="1">
-        <v>126.9858036</v>
+        <v>127.0873411</v>
       </c>
     </row>
     <row r="83">
@@ -1779,10 +1791,10 @@
         <v>84</v>
       </c>
       <c r="B83" s="1">
-        <v>37.5611591</v>
+        <v>37.601757</v>
       </c>
       <c r="C83" s="1">
-        <v>126.994398</v>
+        <v>127.079416</v>
       </c>
     </row>
     <row r="84">
@@ -1790,10 +1802,10 @@
         <v>85</v>
       </c>
       <c r="B84" s="1">
-        <v>37.5592266</v>
+        <v>37.6107683</v>
       </c>
       <c r="C84" s="1">
-        <v>127.005275</v>
+        <v>127.0776921</v>
       </c>
     </row>
     <row r="85">
@@ -1801,10 +1813,10 @@
         <v>86</v>
       </c>
       <c r="B85" s="1">
-        <v>37.5543795</v>
+        <v>37.6191035</v>
       </c>
       <c r="C85" s="1">
-        <v>127.0110164</v>
+        <v>127.0751197</v>
       </c>
     </row>
     <row r="86">
@@ -1812,10 +1824,10 @@
         <v>87</v>
       </c>
       <c r="B86" s="1">
-        <v>37.5550173</v>
+        <v>37.6258623</v>
       </c>
       <c r="C86" s="1">
-        <v>127.0103572</v>
+        <v>127.0728393</v>
       </c>
     </row>
     <row r="87">
@@ -1823,10 +1835,10 @@
         <v>88</v>
       </c>
       <c r="B87" s="1">
-        <v>37.5480381</v>
+        <v>37.6351911</v>
       </c>
       <c r="C87" s="1">
-        <v>127.0158826</v>
+        <v>127.0685438</v>
       </c>
     </row>
     <row r="88">
@@ -1834,10 +1846,10 @@
         <v>89</v>
       </c>
       <c r="B88" s="1">
-        <v>37.5398948</v>
+        <v>37.6425631</v>
       </c>
       <c r="C88" s="1">
-        <v>127.0172208</v>
+        <v>127.0652144</v>
       </c>
     </row>
     <row r="89">
@@ -1845,10 +1857,10 @@
         <v>90</v>
       </c>
       <c r="B89" s="1">
-        <v>37.5235264</v>
+        <v>37.6558674</v>
       </c>
       <c r="C89" s="1">
-        <v>127.0283255</v>
+        <v>127.0619911</v>
       </c>
     </row>
     <row r="90">
@@ -1856,10 +1868,10 @@
         <v>91</v>
       </c>
       <c r="B90" s="1">
-        <v>37.5163915</v>
+        <v>37.6536158</v>
       </c>
       <c r="C90" s="1">
-        <v>127.0203073</v>
+        <v>127.0607581</v>
       </c>
     </row>
     <row r="91">
@@ -1867,10 +1879,10 @@
         <v>92</v>
       </c>
       <c r="B91" s="1">
-        <v>37.5130817999999</v>
+        <v>37.6675895</v>
       </c>
       <c r="C91" s="1">
-        <v>127.0118568</v>
+        <v>127.0569843</v>
       </c>
     </row>
     <row r="92">
@@ -1878,10 +1890,10 @@
         <v>93</v>
       </c>
       <c r="B92" s="1">
-        <v>37.5047736</v>
+        <v>37.6771548</v>
       </c>
       <c r="C92" s="1">
-        <v>127.0049178</v>
+        <v>127.0553068</v>
       </c>
     </row>
     <row r="93">
@@ -1889,10 +1901,10 @@
         <v>94</v>
       </c>
       <c r="B93" s="1">
-        <v>37.4866605</v>
+        <v>37.70008</v>
       </c>
       <c r="C93" s="1">
-        <v>127.0152184</v>
+        <v>127.0531199</v>
       </c>
     </row>
     <row r="94">
@@ -1900,10 +1912,10 @@
         <v>95</v>
       </c>
       <c r="B94" s="1">
-        <v>37.4847605</v>
+        <v>37.6164431</v>
       </c>
       <c r="C94" s="1">
-        <v>127.033371</v>
+        <v>127.0932784</v>
       </c>
     </row>
     <row r="95">
@@ -1911,10 +1923,10 @@
         <v>96</v>
       </c>
       <c r="B95" s="1">
-        <v>37.4869406</v>
+        <v>37.6198541</v>
       </c>
       <c r="C95" s="1">
-        <v>127.0466214</v>
+        <v>127.0832018</v>
       </c>
     </row>
     <row r="96">
@@ -1922,10 +1934,10 @@
         <v>97</v>
       </c>
       <c r="B96" s="1">
-        <v>37.4908245</v>
+        <v>37.6105223</v>
       </c>
       <c r="C96" s="1">
-        <v>127.0553064</v>
+        <v>127.0572772</v>
       </c>
     </row>
     <row r="97">
@@ -1933,10 +1945,10 @@
         <v>98</v>
       </c>
       <c r="B97" s="1">
-        <v>37.4945429</v>
+        <v>37.6062263</v>
       </c>
       <c r="C97" s="1">
-        <v>127.0634256</v>
+        <v>127.0483129</v>
       </c>
     </row>
     <row r="98">
@@ -1944,10 +1956,10 @@
         <v>99</v>
       </c>
       <c r="B98" s="1">
-        <v>37.4966789</v>
+        <v>37.6013813</v>
       </c>
       <c r="C98" s="1">
-        <v>127.0717054</v>
+        <v>127.0411709</v>
       </c>
     </row>
     <row r="99">
@@ -1955,10 +1967,10 @@
         <v>100</v>
       </c>
       <c r="B99" s="1">
-        <v>37.4936861</v>
+        <v>37.5903824</v>
       </c>
       <c r="C99" s="1">
-        <v>127.0794787</v>
+        <v>127.036203</v>
       </c>
     </row>
     <row r="100">
@@ -1966,10 +1978,10 @@
         <v>101</v>
       </c>
       <c r="B100" s="1">
-        <v>37.4839534</v>
+        <v>37.586051</v>
       </c>
       <c r="C100" s="1">
-        <v>127.0844127</v>
+        <v>127.0293623</v>
       </c>
     </row>
     <row r="101">
@@ -1977,10 +1989,10 @@
         <v>102</v>
       </c>
       <c r="B101" s="1">
-        <v>37.4873499</v>
+        <v>37.5791968</v>
       </c>
       <c r="C101" s="1">
-        <v>127.1018416</v>
+        <v>127.0153255</v>
       </c>
     </row>
     <row r="102">
@@ -1988,10 +2000,10 @@
         <v>103</v>
       </c>
       <c r="B102" s="1">
-        <v>37.4928982</v>
+        <v>37.5732808</v>
       </c>
       <c r="C102" s="1">
-        <v>127.1180582</v>
+        <v>127.0166486</v>
       </c>
     </row>
     <row r="103">
@@ -1999,10 +2011,10 @@
         <v>104</v>
       </c>
       <c r="B103" s="1">
-        <v>37.4983224</v>
+        <v>37.5729495</v>
       </c>
       <c r="C103" s="1">
-        <v>127.1256757</v>
+        <v>127.0156058</v>
       </c>
     </row>
     <row r="104">
@@ -2010,10 +2022,10 @@
         <v>105</v>
       </c>
       <c r="B104" s="1">
-        <v>37.5032462</v>
+        <v>37.5652813</v>
       </c>
       <c r="C104" s="1">
-        <v>127.1263422</v>
+        <v>127.0166395</v>
       </c>
     </row>
     <row r="105">
@@ -2021,10 +2033,10 @@
         <v>106</v>
       </c>
       <c r="B105" s="1">
-        <v>37.6705563</v>
+        <v>37.567534</v>
       </c>
       <c r="C105" s="1">
-        <v>127.0793058</v>
+        <v>127.0161118</v>
       </c>
     </row>
     <row r="106">
@@ -2032,10 +2044,10 @@
         <v>107</v>
       </c>
       <c r="B106" s="1">
-        <v>37.6610953</v>
+        <v>37.5603185</v>
       </c>
       <c r="C106" s="1">
-        <v>127.0735256</v>
+        <v>127.0138535</v>
       </c>
     </row>
     <row r="107">
@@ -2043,10 +2055,10 @@
         <v>108</v>
       </c>
       <c r="B107" s="1">
-        <v>37.6558674</v>
+        <v>37.5543795</v>
       </c>
       <c r="C107" s="1">
-        <v>127.0619911</v>
+        <v>127.0110164</v>
       </c>
     </row>
     <row r="108">
@@ -2054,10 +2066,10 @@
         <v>109</v>
       </c>
       <c r="B108" s="1">
-        <v>37.6536158</v>
+        <v>37.5550173</v>
       </c>
       <c r="C108" s="1">
-        <v>127.0607581</v>
+        <v>127.0103572</v>
       </c>
     </row>
     <row r="109">
@@ -2065,10 +2077,10 @@
         <v>110</v>
       </c>
       <c r="B109" s="1">
-        <v>37.6531856</v>
+        <v>37.5481325</v>
       </c>
       <c r="C109" s="1">
-        <v>127.0481139</v>
+        <v>127.0070317</v>
       </c>
     </row>
     <row r="110">
@@ -2076,10 +2088,10 @@
         <v>111</v>
       </c>
       <c r="B110" s="1">
-        <v>37.6488107</v>
+        <v>37.5407506</v>
       </c>
       <c r="C110" s="1">
-        <v>127.034866</v>
+        <v>127.001835</v>
       </c>
     </row>
     <row r="111">
@@ -2087,10 +2099,10 @@
         <v>112</v>
       </c>
       <c r="B111" s="1">
-        <v>37.6397753</v>
+        <v>37.5345103</v>
       </c>
       <c r="C111" s="1">
-        <v>127.0272077</v>
+        <v>126.9946564</v>
       </c>
     </row>
     <row r="112">
@@ -2098,10 +2110,10 @@
         <v>113</v>
       </c>
       <c r="B112" s="1">
-        <v>37.6298777</v>
+        <v>37.5347918999999</v>
       </c>
       <c r="C112" s="1">
-        <v>127.0247141</v>
+        <v>126.9870163</v>
       </c>
     </row>
     <row r="113">
@@ -2109,10 +2121,10 @@
         <v>114</v>
       </c>
       <c r="B113" s="1">
-        <v>37.6151041</v>
+        <v>37.5343935</v>
       </c>
       <c r="C113" s="1">
-        <v>127.0300461</v>
+        <v>126.9730142</v>
       </c>
     </row>
     <row r="114">
@@ -2120,10 +2132,10 @@
         <v>115</v>
       </c>
       <c r="B114" s="1">
-        <v>37.6032254</v>
+        <v>37.5477312</v>
       </c>
       <c r="C114" s="1">
-        <v>127.0249647</v>
+        <v>126.9423543</v>
       </c>
     </row>
     <row r="115">
@@ -2131,10 +2143,10 @@
         <v>116</v>
       </c>
       <c r="B115" s="1">
-        <v>37.5930482</v>
+        <v>37.5474463</v>
       </c>
       <c r="C115" s="1">
-        <v>127.0167136</v>
+        <v>126.9319256</v>
       </c>
     </row>
     <row r="116">
@@ -2142,10 +2154,10 @@
         <v>117</v>
       </c>
       <c r="B116" s="1">
-        <v>37.5880209</v>
+        <v>37.5466338</v>
       </c>
       <c r="C116" s="1">
-        <v>127.0057966</v>
+        <v>126.9226203</v>
       </c>
     </row>
     <row r="117">
@@ -2153,10 +2165,10 @@
         <v>118</v>
       </c>
       <c r="B117" s="1">
-        <v>37.581893</v>
+        <v>37.5500076999999</v>
       </c>
       <c r="C117" s="1">
-        <v>127.0019528</v>
+        <v>126.9145039</v>
       </c>
     </row>
     <row r="118">
@@ -2164,10 +2176,10 @@
         <v>119</v>
       </c>
       <c r="B118" s="1">
-        <v>37.5608222</v>
+        <v>37.5489656</v>
       </c>
       <c r="C118" s="1">
-        <v>126.9853555</v>
+        <v>126.9134767</v>
       </c>
     </row>
     <row r="119">
@@ -2175,10 +2187,10 @@
         <v>120</v>
       </c>
       <c r="B119" s="1">
-        <v>37.5590295</v>
+        <v>37.5557572</v>
       </c>
       <c r="C119" s="1">
-        <v>126.9772521</v>
+        <v>126.909907</v>
       </c>
     </row>
     <row r="120">
@@ -2186,10 +2198,10 @@
         <v>121</v>
       </c>
       <c r="B120" s="1">
-        <v>37.5530656</v>
+        <v>37.5649979</v>
       </c>
       <c r="C120" s="1">
-        <v>126.9727965</v>
+        <v>126.9015161</v>
       </c>
     </row>
     <row r="121">
@@ -2197,10 +2209,10 @@
         <v>122</v>
       </c>
       <c r="B121" s="1">
-        <v>37.5455275</v>
+        <v>37.5693111</v>
       </c>
       <c r="C121" s="1">
-        <v>126.9719697</v>
+        <v>126.8992963</v>
       </c>
     </row>
     <row r="122">
@@ -2208,10 +2220,10 @@
         <v>123</v>
       </c>
       <c r="B122" s="1">
-        <v>37.5343935</v>
+        <v>37.5836921</v>
       </c>
       <c r="C122" s="1">
-        <v>126.9730142</v>
+        <v>126.9092563</v>
       </c>
     </row>
     <row r="123">
@@ -2219,10 +2231,10 @@
         <v>124</v>
       </c>
       <c r="B123" s="1">
-        <v>37.5293642</v>
+        <v>37.5910797</v>
       </c>
       <c r="C123" s="1">
-        <v>126.9682985</v>
+        <v>126.9132724</v>
       </c>
     </row>
     <row r="124">
@@ -2230,10 +2242,10 @@
         <v>125</v>
       </c>
       <c r="B124" s="1">
-        <v>37.5224811</v>
+        <v>37.6111396</v>
       </c>
       <c r="C124" s="1">
-        <v>126.9736707</v>
+        <v>126.9169368</v>
       </c>
     </row>
     <row r="125">
@@ -2241,10 +2253,10 @@
         <v>126</v>
       </c>
       <c r="B125" s="1">
-        <v>37.5034646999999</v>
+        <v>37.6188881</v>
       </c>
       <c r="C125" s="1">
-        <v>126.9799265</v>
+        <v>126.920832</v>
       </c>
     </row>
     <row r="126">
@@ -2252,10 +2264,10 @@
         <v>127</v>
       </c>
       <c r="B126" s="1">
-        <v>37.4875138</v>
+        <v>37.6182636</v>
       </c>
       <c r="C126" s="1">
-        <v>126.9821618</v>
+        <v>126.9329115</v>
       </c>
     </row>
     <row r="127">
@@ -2263,10 +2275,10 @@
         <v>128</v>
       </c>
       <c r="B127" s="1">
-        <v>37.4643638</v>
+        <v>37.6104829</v>
       </c>
       <c r="C127" s="1">
-        <v>126.9892695</v>
+        <v>126.9292884</v>
       </c>
     </row>
     <row r="128">
@@ -2274,10 +2286,10 @@
         <v>129</v>
       </c>
       <c r="B128" s="1">
-        <v>37.5176664</v>
+        <v>37.6059994</v>
       </c>
       <c r="C128" s="1">
-        <v>126.9146626</v>
+        <v>126.9229527</v>
       </c>
     </row>
     <row r="129">
@@ -2285,10 +2297,10 @@
         <v>130</v>
       </c>
       <c r="B129" s="1">
-        <v>37.4809056</v>
+        <v>37.5989284</v>
       </c>
       <c r="C129" s="1">
-        <v>126.8828399</v>
+        <v>126.9154095</v>
       </c>
     </row>
     <row r="130">
@@ -2296,10 +2308,10 @@
         <v>131</v>
       </c>
       <c r="B130" s="1">
-        <v>37.4922113</v>
+        <v>37.4943114999999</v>
       </c>
       <c r="C130" s="1">
-        <v>126.823298</v>
+        <v>127.1518299</v>
       </c>
     </row>
     <row r="131">
@@ -2307,10 +2319,10 @@
         <v>132</v>
       </c>
       <c r="B131" s="1">
-        <v>37.6152323</v>
+        <v>37.4942493</v>
       </c>
       <c r="C131" s="1">
-        <v>127.066831</v>
+        <v>127.1419784</v>
       </c>
     </row>
     <row r="132">
@@ -2318,10 +2330,10 @@
         <v>133</v>
       </c>
       <c r="B132" s="1">
-        <v>37.6890803</v>
+        <v>37.4979912</v>
       </c>
       <c r="C132" s="1">
-        <v>127.046509</v>
+        <v>127.135763</v>
       </c>
     </row>
     <row r="133">
@@ -2329,10 +2341,10 @@
         <v>134</v>
       </c>
       <c r="B133" s="1">
-        <v>37.517161</v>
+        <v>37.5032462</v>
       </c>
       <c r="C133" s="1">
-        <v>127.041288</v>
+        <v>127.1263422</v>
       </c>
     </row>
     <row r="134">
@@ -2340,10 +2352,10 @@
         <v>135</v>
       </c>
       <c r="B134" s="1">
-        <v>37.4398574</v>
+        <v>37.50828</v>
       </c>
       <c r="C134" s="1">
-        <v>127.1276594</v>
+        <v>127.1256705</v>
       </c>
     </row>
     <row r="135">
@@ -2351,10 +2363,10 @@
         <v>136</v>
       </c>
       <c r="B135" s="1">
-        <v>37.5959947</v>
+        <v>37.5277926</v>
       </c>
       <c r="C135" s="1">
-        <v>127.0843699</v>
+        <v>127.1362463</v>
       </c>
     </row>
     <row r="136">
@@ -2362,10 +2374,10 @@
         <v>137</v>
       </c>
       <c r="B136" s="1">
-        <v>37.5251429</v>
+        <v>37.5528183</v>
       </c>
       <c r="C136" s="1">
-        <v>126.8860734</v>
+        <v>127.1568023</v>
       </c>
     </row>
     <row r="137">
@@ -2373,10 +2385,10 @@
         <v>138</v>
       </c>
       <c r="B137" s="1">
-        <v>37.5394453</v>
+        <v>37.5556248</v>
       </c>
       <c r="C137" s="1">
-        <v>126.9611372</v>
+        <v>127.1538766</v>
       </c>
     </row>
     <row r="138">
@@ -2384,10 +2396,10 @@
         <v>139</v>
       </c>
       <c r="B138" s="1">
-        <v>37.5444535</v>
+        <v>37.5513169</v>
       </c>
       <c r="C138" s="1">
-        <v>126.9511752</v>
+        <v>127.1439955</v>
       </c>
     </row>
     <row r="139">
@@ -2395,10 +2407,10 @@
         <v>140</v>
       </c>
       <c r="B139" s="1">
-        <v>37.5768989</v>
+        <v>37.5460635</v>
       </c>
       <c r="C139" s="1">
-        <v>126.9016424</v>
+        <v>127.1430959</v>
       </c>
     </row>
     <row r="140">
@@ -2406,10 +2418,10 @@
         <v>141</v>
       </c>
       <c r="B140" s="1">
-        <v>37.5772156</v>
+        <v>37.5383746</v>
       </c>
       <c r="C140" s="1">
-        <v>126.8126263</v>
+        <v>127.1402046</v>
       </c>
     </row>
     <row r="141">
@@ -2417,10 +2429,10 @@
         <v>142</v>
       </c>
       <c r="B141" s="1">
-        <v>37.5722225</v>
+        <v>37.5356923999999</v>
       </c>
       <c r="C141" s="1">
-        <v>126.8059564</v>
+        <v>127.1340676</v>
       </c>
     </row>
     <row r="142">
@@ -2428,10 +2440,10 @@
         <v>143</v>
       </c>
       <c r="B142" s="1">
-        <v>37.5667733</v>
+        <v>37.5451442</v>
       </c>
       <c r="C142" s="1">
-        <v>126.8025118</v>
+        <v>127.103499</v>
       </c>
     </row>
     <row r="143">
@@ -2439,10 +2451,10 @@
         <v>144</v>
       </c>
       <c r="B143" s="1">
-        <v>37.561401</v>
+        <v>37.5528109</v>
       </c>
       <c r="C143" s="1">
-        <v>126.810935</v>
+        <v>127.0889706</v>
       </c>
     </row>
     <row r="144">
@@ -2450,10 +2462,10 @@
         <v>145</v>
       </c>
       <c r="B144" s="1">
-        <v>37.5602741999999</v>
+        <v>37.5614626</v>
       </c>
       <c r="C144" s="1">
-        <v>126.8250127</v>
+        <v>127.0644199</v>
       </c>
     </row>
     <row r="145">
@@ -2461,10 +2473,10 @@
         <v>146</v>
       </c>
       <c r="B145" s="1">
-        <v>37.5589471</v>
+        <v>37.5668422</v>
       </c>
       <c r="C145" s="1">
-        <v>126.8372198</v>
+        <v>127.0526017</v>
       </c>
     </row>
     <row r="146">
@@ -2472,10 +2484,10 @@
         <v>147</v>
       </c>
       <c r="B146" s="1">
-        <v>37.5491827</v>
+        <v>37.5660505</v>
       </c>
       <c r="C146" s="1">
-        <v>126.8364006</v>
+        <v>127.0429223</v>
       </c>
     </row>
     <row r="147">
@@ -2483,10 +2495,10 @@
         <v>148</v>
       </c>
       <c r="B147" s="1">
-        <v>37.5410793</v>
+        <v>37.5573015</v>
       </c>
       <c r="C147" s="1">
-        <v>126.8408434</v>
+        <v>127.0294648</v>
       </c>
     </row>
     <row r="148">
@@ -2494,10 +2506,10 @@
         <v>149</v>
       </c>
       <c r="B148" s="1">
-        <v>37.5325506</v>
+        <v>37.5548998</v>
       </c>
       <c r="C148" s="1">
-        <v>126.8463214</v>
+        <v>127.0199234</v>
       </c>
     </row>
     <row r="149">
@@ -2505,10 +2517,10 @@
         <v>150</v>
       </c>
       <c r="B149" s="1">
-        <v>37.5246352</v>
+        <v>37.5657177</v>
       </c>
       <c r="C149" s="1">
-        <v>126.8536475</v>
+        <v>127.0084849</v>
       </c>
     </row>
     <row r="150">
@@ -2516,10 +2528,10 @@
         <v>151</v>
       </c>
       <c r="B150" s="1">
-        <v>37.52606</v>
+        <v>37.5644784</v>
       </c>
       <c r="C150" s="1">
-        <v>126.8654311</v>
+        <v>127.0071588</v>
       </c>
     </row>
     <row r="151">
@@ -2527,10 +2539,10 @@
         <v>152</v>
       </c>
       <c r="B151" s="1">
-        <v>37.5246</v>
+        <v>37.5645651</v>
       </c>
       <c r="C151" s="1">
-        <v>126.8743362</v>
+        <v>127.0062216</v>
       </c>
     </row>
     <row r="152">
@@ -2538,10 +2550,10 @@
         <v>153</v>
       </c>
       <c r="B152" s="1">
-        <v>37.5226937</v>
+        <v>37.5664887999999</v>
       </c>
       <c r="C152" s="1">
-        <v>126.9049377</v>
+        <v>126.996528</v>
       </c>
     </row>
     <row r="153">
@@ -2549,10 +2561,10 @@
         <v>154</v>
       </c>
       <c r="B153" s="1">
-        <v>37.5235124</v>
+        <v>37.5661417</v>
       </c>
       <c r="C153" s="1">
-        <v>126.9264939</v>
+        <v>126.9985136</v>
       </c>
     </row>
     <row r="154">
@@ -2560,10 +2572,10 @@
         <v>155</v>
       </c>
       <c r="B154" s="1">
-        <v>37.5267506</v>
+        <v>37.5703842</v>
       </c>
       <c r="C154" s="1">
-        <v>126.9328452</v>
+        <v>126.9920077</v>
       </c>
     </row>
     <row r="155">
@@ -2571,10 +2583,10 @@
         <v>156</v>
       </c>
       <c r="B155" s="1">
-        <v>37.5397244</v>
+        <v>37.5711966</v>
       </c>
       <c r="C155" s="1">
-        <v>126.9459616</v>
+        <v>126.9919594</v>
       </c>
     </row>
     <row r="156">
@@ -2582,10 +2594,10 @@
         <v>157</v>
       </c>
       <c r="B156" s="1">
-        <v>37.5513892</v>
+        <v>37.5715436</v>
       </c>
       <c r="C156" s="1">
-        <v>126.9556875</v>
+        <v>126.9772067</v>
       </c>
     </row>
     <row r="157">
@@ -2604,10 +2616,10 @@
         <v>159</v>
       </c>
       <c r="B158" s="1">
-        <v>37.5715436</v>
+        <v>37.5594926</v>
       </c>
       <c r="C158" s="1">
-        <v>126.9772067</v>
+        <v>126.9638176</v>
       </c>
     </row>
     <row r="159">
@@ -2615,10 +2627,10 @@
         <v>160</v>
       </c>
       <c r="B159" s="1">
-        <v>37.5603185</v>
+        <v>37.5611255</v>
       </c>
       <c r="C159" s="1">
-        <v>127.0138535</v>
+        <v>126.9635279</v>
       </c>
     </row>
     <row r="160">
@@ -2626,10 +2638,10 @@
         <v>161</v>
       </c>
       <c r="B160" s="1">
-        <v>37.5548998</v>
+        <v>37.5513892</v>
       </c>
       <c r="C160" s="1">
-        <v>127.0199234</v>
+        <v>126.9556875</v>
       </c>
     </row>
     <row r="161">
@@ -2637,10 +2649,10 @@
         <v>162</v>
       </c>
       <c r="B161" s="1">
-        <v>37.5573015</v>
+        <v>37.5397244</v>
       </c>
       <c r="C161" s="1">
-        <v>127.0294648</v>
+        <v>126.9459616</v>
       </c>
     </row>
     <row r="162">
@@ -2648,10 +2660,10 @@
         <v>163</v>
       </c>
       <c r="B162" s="1">
-        <v>37.5660505</v>
+        <v>37.5267506</v>
       </c>
       <c r="C162" s="1">
-        <v>127.0429223</v>
+        <v>126.9328452</v>
       </c>
     </row>
     <row r="163">
@@ -2659,10 +2671,10 @@
         <v>164</v>
       </c>
       <c r="B163" s="1">
-        <v>37.5668422</v>
+        <v>37.5226937</v>
       </c>
       <c r="C163" s="1">
-        <v>127.0526017</v>
+        <v>126.9049377</v>
       </c>
     </row>
     <row r="164">
@@ -2670,10 +2682,10 @@
         <v>165</v>
       </c>
       <c r="B164" s="1">
-        <v>37.5614626</v>
+        <v>37.5256563</v>
       </c>
       <c r="C164" s="1">
-        <v>127.0644199</v>
+        <v>126.8966142</v>
       </c>
     </row>
     <row r="165">
@@ -2681,10 +2693,10 @@
         <v>166</v>
       </c>
       <c r="B165" s="1">
-        <v>37.5569984</v>
+        <v>37.5243614</v>
       </c>
       <c r="C165" s="1">
-        <v>127.079719</v>
+        <v>126.894287</v>
       </c>
     </row>
     <row r="166">
@@ -2692,10 +2704,10 @@
         <v>167</v>
       </c>
       <c r="B166" s="1">
-        <v>37.5528109</v>
+        <v>37.5246</v>
       </c>
       <c r="C166" s="1">
-        <v>127.0889706</v>
+        <v>126.8743362</v>
       </c>
     </row>
     <row r="167">
@@ -2703,10 +2715,10 @@
         <v>168</v>
       </c>
       <c r="B167" s="1">
-        <v>37.5451442</v>
+        <v>37.52606</v>
       </c>
       <c r="C167" s="1">
-        <v>127.103499</v>
+        <v>126.8654311</v>
       </c>
     </row>
     <row r="168">
@@ -2714,10 +2726,10 @@
         <v>169</v>
       </c>
       <c r="B168" s="1">
-        <v>37.5384618</v>
+        <v>37.5246352</v>
       </c>
       <c r="C168" s="1">
-        <v>127.1250941</v>
+        <v>126.8536475</v>
       </c>
     </row>
     <row r="169">
@@ -2725,10 +2737,10 @@
         <v>170</v>
       </c>
       <c r="B169" s="1">
-        <v>37.5356923999999</v>
+        <v>37.5325506</v>
       </c>
       <c r="C169" s="1">
-        <v>127.1340676</v>
+        <v>126.8463214</v>
       </c>
     </row>
     <row r="170">
@@ -2736,10 +2748,10 @@
         <v>171</v>
       </c>
       <c r="B170" s="1">
-        <v>37.5383746</v>
+        <v>37.5410793</v>
       </c>
       <c r="C170" s="1">
-        <v>127.1402046</v>
+        <v>126.8408434</v>
       </c>
     </row>
     <row r="171">
@@ -2747,10 +2759,10 @@
         <v>172</v>
       </c>
       <c r="B171" s="1">
-        <v>37.5460635</v>
+        <v>37.5491827</v>
       </c>
       <c r="C171" s="1">
-        <v>127.1430959</v>
+        <v>126.8364006</v>
       </c>
     </row>
     <row r="172">
@@ -2758,10 +2770,10 @@
         <v>173</v>
       </c>
       <c r="B172" s="1">
-        <v>37.5513169</v>
+        <v>37.5589471</v>
       </c>
       <c r="C172" s="1">
-        <v>127.1439955</v>
+        <v>126.8372198</v>
       </c>
     </row>
     <row r="173">
@@ -2769,10 +2781,10 @@
         <v>174</v>
       </c>
       <c r="B173" s="1">
-        <v>37.5556248</v>
+        <v>37.5602741999999</v>
       </c>
       <c r="C173" s="1">
-        <v>127.1538766</v>
+        <v>126.8250127</v>
       </c>
     </row>
     <row r="174">
@@ -2780,10 +2792,10 @@
         <v>175</v>
       </c>
       <c r="B174" s="1">
-        <v>37.5528183</v>
+        <v>37.561401</v>
       </c>
       <c r="C174" s="1">
-        <v>127.1568023</v>
+        <v>126.810935</v>
       </c>
     </row>
     <row r="175">
@@ -2791,10 +2803,10 @@
         <v>176</v>
       </c>
       <c r="B175" s="1">
-        <v>37.5277926</v>
+        <v>37.5722225</v>
       </c>
       <c r="C175" s="1">
-        <v>127.1362463</v>
+        <v>126.8059564</v>
       </c>
     </row>
     <row r="176">
@@ -2802,10 +2814,10 @@
         <v>177</v>
       </c>
       <c r="B176" s="1">
-        <v>37.5164494</v>
+        <v>37.5772156</v>
       </c>
       <c r="C176" s="1">
-        <v>127.1311068</v>
+        <v>126.8126263</v>
       </c>
     </row>
     <row r="177">
@@ -2813,10 +2825,10 @@
         <v>178</v>
       </c>
       <c r="B177" s="1">
-        <v>37.50828</v>
+        <v>37.4643638</v>
       </c>
       <c r="C177" s="1">
-        <v>127.1256705</v>
+        <v>126.9892695</v>
       </c>
     </row>
     <row r="178">
@@ -2824,10 +2836,10 @@
         <v>179</v>
       </c>
       <c r="B178" s="1">
-        <v>37.4979912</v>
+        <v>37.4764838</v>
       </c>
       <c r="C178" s="1">
-        <v>127.135763</v>
+        <v>126.9813957</v>
       </c>
     </row>
     <row r="179">
@@ -2835,10 +2847,10 @@
         <v>180</v>
       </c>
       <c r="B179" s="1">
-        <v>37.4942493</v>
+        <v>37.4771295</v>
       </c>
       <c r="C179" s="1">
-        <v>127.1419784</v>
+        <v>126.9816651</v>
       </c>
     </row>
     <row r="180">
@@ -2846,10 +2858,10 @@
         <v>181</v>
       </c>
       <c r="B180" s="1">
-        <v>37.4943114999999</v>
+        <v>37.4875138</v>
       </c>
       <c r="C180" s="1">
-        <v>127.1518299</v>
+        <v>126.9821618</v>
       </c>
     </row>
     <row r="181">
@@ -2857,10 +2869,10 @@
         <v>182</v>
       </c>
       <c r="B181" s="1">
-        <v>37.5989284</v>
+        <v>37.5293642</v>
       </c>
       <c r="C181" s="1">
-        <v>126.9154095</v>
+        <v>126.9682985</v>
       </c>
     </row>
     <row r="182">
@@ -2868,10 +2880,10 @@
         <v>183</v>
       </c>
       <c r="B182" s="1">
-        <v>37.6059994</v>
+        <v>37.5455275</v>
       </c>
       <c r="C182" s="1">
-        <v>126.9229527</v>
+        <v>126.9719697</v>
       </c>
     </row>
     <row r="183">
@@ -2879,10 +2891,10 @@
         <v>184</v>
       </c>
       <c r="B183" s="1">
-        <v>37.6182636</v>
+        <v>37.5590295</v>
       </c>
       <c r="C183" s="1">
-        <v>126.9329115</v>
+        <v>126.9772521</v>
       </c>
     </row>
     <row r="184">
@@ -2890,10 +2902,10 @@
         <v>185</v>
       </c>
       <c r="B184" s="1">
-        <v>37.6111396</v>
+        <v>37.5608222</v>
       </c>
       <c r="C184" s="1">
-        <v>126.9169368</v>
+        <v>126.9853555</v>
       </c>
     </row>
     <row r="185">
@@ -2901,21 +2913,21 @@
         <v>186</v>
       </c>
       <c r="B185" s="1">
-        <v>37.5910797</v>
+        <v>37.5611591</v>
       </c>
       <c r="C185" s="1">
-        <v>126.9132724</v>
+        <v>126.994398</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B186" s="1">
-        <v>37.5836921</v>
-      </c>
-      <c r="C186" s="1">
-        <v>126.9092563</v>
+      <c r="B186" s="2">
+        <v>37.571747</v>
+      </c>
+      <c r="C186" s="2">
+        <v>127.011172</v>
       </c>
     </row>
     <row r="187">
@@ -2923,10 +2935,10 @@
         <v>188</v>
       </c>
       <c r="B187" s="1">
-        <v>37.5693111</v>
+        <v>37.5703848</v>
       </c>
       <c r="C187" s="1">
-        <v>126.8992963</v>
+        <v>127.009529</v>
       </c>
     </row>
     <row r="188">
@@ -2934,10 +2946,10 @@
         <v>189</v>
       </c>
       <c r="B188" s="1">
-        <v>37.5649979</v>
+        <v>37.581893</v>
       </c>
       <c r="C188" s="1">
-        <v>126.9015161</v>
+        <v>127.0019528</v>
       </c>
     </row>
     <row r="189">
@@ -2945,10 +2957,10 @@
         <v>190</v>
       </c>
       <c r="B189" s="1">
-        <v>37.5557572</v>
+        <v>37.5880209</v>
       </c>
       <c r="C189" s="1">
-        <v>126.909907</v>
+        <v>127.0057966</v>
       </c>
     </row>
     <row r="190">
@@ -2956,10 +2968,10 @@
         <v>191</v>
       </c>
       <c r="B190" s="1">
-        <v>37.5466338</v>
+        <v>37.6032254</v>
       </c>
       <c r="C190" s="1">
-        <v>126.9226203</v>
+        <v>127.0249647</v>
       </c>
     </row>
     <row r="191">
@@ -2967,10 +2979,10 @@
         <v>192</v>
       </c>
       <c r="B191" s="1">
-        <v>37.5474463</v>
+        <v>37.6151041</v>
       </c>
       <c r="C191" s="1">
-        <v>126.9319256</v>
+        <v>127.0300461</v>
       </c>
     </row>
     <row r="192">
@@ -2978,10 +2990,10 @@
         <v>193</v>
       </c>
       <c r="B192" s="1">
-        <v>37.5477312</v>
+        <v>37.6298777</v>
       </c>
       <c r="C192" s="1">
-        <v>126.9423543</v>
+        <v>127.0247141</v>
       </c>
     </row>
     <row r="193">
@@ -2989,10 +3001,10 @@
         <v>194</v>
       </c>
       <c r="B193" s="1">
-        <v>37.5347918999999</v>
+        <v>37.6397753</v>
       </c>
       <c r="C193" s="1">
-        <v>126.9870163</v>
+        <v>127.0272077</v>
       </c>
     </row>
     <row r="194">
@@ -3000,10 +3012,10 @@
         <v>195</v>
       </c>
       <c r="B194" s="1">
-        <v>37.5345103</v>
+        <v>37.6488107</v>
       </c>
       <c r="C194" s="1">
-        <v>126.9946564</v>
+        <v>127.034866</v>
       </c>
     </row>
     <row r="195">
@@ -3011,10 +3023,10 @@
         <v>196</v>
       </c>
       <c r="B195" s="1">
-        <v>37.5407506</v>
+        <v>37.6531856</v>
       </c>
       <c r="C195" s="1">
-        <v>127.001835</v>
+        <v>127.0481139</v>
       </c>
     </row>
     <row r="196">
@@ -3022,10 +3034,10 @@
         <v>197</v>
       </c>
       <c r="B196" s="1">
-        <v>37.5481325</v>
+        <v>37.6610953</v>
       </c>
       <c r="C196" s="1">
-        <v>127.0070317</v>
+        <v>127.0735256</v>
       </c>
     </row>
     <row r="197">
@@ -3033,10 +3045,10 @@
         <v>198</v>
       </c>
       <c r="B197" s="1">
-        <v>37.5791968</v>
+        <v>37.6705563</v>
       </c>
       <c r="C197" s="1">
-        <v>127.0153255</v>
+        <v>127.0793058</v>
       </c>
     </row>
     <row r="198">
@@ -3044,10 +3056,10 @@
         <v>199</v>
       </c>
       <c r="B198" s="1">
-        <v>37.5855633</v>
+        <v>37.4983224</v>
       </c>
       <c r="C198" s="1">
-        <v>127.0201782</v>
+        <v>127.1256757</v>
       </c>
     </row>
     <row r="199">
@@ -3055,10 +3067,10 @@
         <v>200</v>
       </c>
       <c r="B199" s="1">
-        <v>37.586051</v>
+        <v>37.4873499</v>
       </c>
       <c r="C199" s="1">
-        <v>127.0293623</v>
+        <v>127.1018416</v>
       </c>
     </row>
     <row r="200">
@@ -3066,10 +3078,10 @@
         <v>201</v>
       </c>
       <c r="B200" s="1">
-        <v>37.5903824</v>
+        <v>37.4839534</v>
       </c>
       <c r="C200" s="1">
-        <v>127.036203</v>
+        <v>127.0844127</v>
       </c>
     </row>
     <row r="201">
@@ -3077,10 +3089,10 @@
         <v>202</v>
       </c>
       <c r="B201" s="1">
-        <v>37.6013813</v>
+        <v>37.4936861</v>
       </c>
       <c r="C201" s="1">
-        <v>127.0411709</v>
+        <v>127.0794787</v>
       </c>
     </row>
     <row r="202">
@@ -3088,10 +3100,10 @@
         <v>203</v>
       </c>
       <c r="B202" s="1">
-        <v>37.6062263</v>
+        <v>37.4966789</v>
       </c>
       <c r="C202" s="1">
-        <v>127.0483129</v>
+        <v>127.0717054</v>
       </c>
     </row>
     <row r="203">
@@ -3099,10 +3111,10 @@
         <v>204</v>
       </c>
       <c r="B203" s="1">
-        <v>37.6105223</v>
+        <v>37.4945429</v>
       </c>
       <c r="C203" s="1">
-        <v>127.0572772</v>
+        <v>127.0634256</v>
       </c>
     </row>
     <row r="204">
@@ -3110,10 +3122,10 @@
         <v>205</v>
       </c>
       <c r="B204" s="1">
-        <v>37.6191035</v>
+        <v>37.4908245</v>
       </c>
       <c r="C204" s="1">
-        <v>127.0751197</v>
+        <v>127.0553064</v>
       </c>
     </row>
     <row r="205">
@@ -3121,10 +3133,10 @@
         <v>206</v>
       </c>
       <c r="B205" s="1">
-        <v>37.6198541</v>
+        <v>37.4869406</v>
       </c>
       <c r="C205" s="1">
-        <v>127.0832018</v>
+        <v>127.0466214</v>
       </c>
     </row>
     <row r="206">
@@ -3132,10 +3144,10 @@
         <v>207</v>
       </c>
       <c r="B206" s="1">
-        <v>37.6164431</v>
+        <v>37.4847605</v>
       </c>
       <c r="C206" s="1">
-        <v>127.0932784</v>
+        <v>127.033371</v>
       </c>
     </row>
     <row r="207">
@@ -3143,10 +3155,10 @@
         <v>208</v>
       </c>
       <c r="B207" s="1">
-        <v>37.70008</v>
+        <v>37.4866605</v>
       </c>
       <c r="C207" s="1">
-        <v>127.0531199</v>
+        <v>127.0152184</v>
       </c>
     </row>
     <row r="208">
@@ -3154,10 +3166,10 @@
         <v>209</v>
       </c>
       <c r="B208" s="1">
-        <v>37.6771548</v>
+        <v>37.5130817999999</v>
       </c>
       <c r="C208" s="1">
-        <v>127.0553068</v>
+        <v>127.0118568</v>
       </c>
     </row>
     <row r="209">
@@ -3165,10 +3177,10 @@
         <v>210</v>
       </c>
       <c r="B209" s="1">
-        <v>37.6675895</v>
+        <v>37.5163915</v>
       </c>
       <c r="C209" s="1">
-        <v>127.0569843</v>
+        <v>127.0203073</v>
       </c>
     </row>
     <row r="210">
@@ -3176,10 +3188,10 @@
         <v>211</v>
       </c>
       <c r="B210" s="1">
-        <v>37.6425631</v>
+        <v>37.5235264</v>
       </c>
       <c r="C210" s="1">
-        <v>127.0652144</v>
+        <v>127.0283255</v>
       </c>
     </row>
     <row r="211">
@@ -3187,10 +3199,10 @@
         <v>212</v>
       </c>
       <c r="B211" s="1">
-        <v>37.6351911</v>
+        <v>37.5480381</v>
       </c>
       <c r="C211" s="1">
-        <v>127.0685438</v>
+        <v>127.0158826</v>
       </c>
     </row>
     <row r="212">
@@ -3198,10 +3210,10 @@
         <v>213</v>
       </c>
       <c r="B212" s="1">
-        <v>37.6258623</v>
+        <v>37.5592266</v>
       </c>
       <c r="C212" s="1">
-        <v>127.0728393</v>
+        <v>127.005275</v>
       </c>
     </row>
     <row r="213">
@@ -3209,10 +3221,10 @@
         <v>214</v>
       </c>
       <c r="B213" s="1">
-        <v>37.6107683</v>
+        <v>37.56617</v>
       </c>
       <c r="C213" s="1">
-        <v>127.0776921</v>
+        <v>126.9902025</v>
       </c>
     </row>
     <row r="214">
@@ -3220,10 +3232,10 @@
         <v>215</v>
       </c>
       <c r="B214" s="1">
-        <v>37.601757</v>
+        <v>37.5664121</v>
       </c>
       <c r="C214" s="1">
-        <v>127.079416</v>
+        <v>126.9941848</v>
       </c>
     </row>
     <row r="215">
@@ -3231,10 +3243,10 @@
         <v>216</v>
       </c>
       <c r="B215" s="1">
-        <v>37.5891527</v>
+        <v>37.576696</v>
       </c>
       <c r="C215" s="1">
-        <v>127.0873411</v>
+        <v>126.9858036</v>
       </c>
     </row>
     <row r="216">
@@ -3242,10 +3254,10 @@
         <v>217</v>
       </c>
       <c r="B216" s="1">
-        <v>37.5817877</v>
+        <v>37.5758199</v>
       </c>
       <c r="C216" s="1">
-        <v>127.0843345</v>
+        <v>126.9730579</v>
       </c>
     </row>
     <row r="217">
@@ -3253,10 +3265,10 @@
         <v>218</v>
       </c>
       <c r="B217" s="1">
-        <v>37.5734436</v>
+        <v>37.5743009</v>
       </c>
       <c r="C217" s="1">
-        <v>127.0864823</v>
+        <v>126.9559178</v>
       </c>
     </row>
     <row r="218">
@@ -3264,10 +3276,10 @@
         <v>219</v>
       </c>
       <c r="B218" s="1">
-        <v>37.5657147</v>
+        <v>37.5823607</v>
       </c>
       <c r="C218" s="1">
-        <v>127.0841917</v>
+        <v>126.9504375</v>
       </c>
     </row>
     <row r="219">
@@ -3275,21 +3287,21 @@
         <v>220</v>
       </c>
       <c r="B219" s="1">
-        <v>37.5471128999999</v>
+        <v>37.5872664</v>
       </c>
       <c r="C219" s="1">
-        <v>127.0739401</v>
+        <v>126.9458373</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B220" s="1">
-        <v>37.5319161</v>
-      </c>
-      <c r="C220" s="1">
-        <v>127.0669943</v>
+      <c r="B220" s="2">
+        <v>37.600716</v>
+      </c>
+      <c r="C220" s="2">
+        <v>126.936004</v>
       </c>
     </row>
     <row r="221">
@@ -3297,10 +3309,10 @@
         <v>222</v>
       </c>
       <c r="B221" s="1">
-        <v>37.5191066</v>
+        <v>37.6375367</v>
       </c>
       <c r="C221" s="1">
-        <v>127.0520336</v>
+        <v>126.9185875</v>
       </c>
     </row>
     <row r="222">
@@ -3308,10 +3320,10 @@
         <v>223</v>
       </c>
       <c r="B222" s="1">
-        <v>37.5111584</v>
+        <v>37.6487977</v>
       </c>
       <c r="C222" s="1">
-        <v>127.0216392</v>
+        <v>126.9108511</v>
       </c>
     </row>
     <row r="223">
@@ -3319,10 +3331,10 @@
         <v>224</v>
       </c>
       <c r="B223" s="1">
-        <v>37.5103093</v>
+        <v>37.5738576</v>
       </c>
       <c r="C223" s="1">
-        <v>127.0218222</v>
+        <v>127.0379896</v>
       </c>
     </row>
     <row r="224">
@@ -3330,10 +3342,10 @@
         <v>225</v>
       </c>
       <c r="B224" s="1">
-        <v>37.508249</v>
+        <v>37.5182935</v>
       </c>
       <c r="C224" s="1">
-        <v>127.0118029</v>
+        <v>126.8536189</v>
       </c>
     </row>
     <row r="225">
@@ -3341,10 +3353,10 @@
         <v>226</v>
       </c>
       <c r="B225" s="1">
-        <v>37.4882577</v>
+        <v>37.5125175</v>
       </c>
       <c r="C225" s="1">
-        <v>126.9931587</v>
+        <v>126.8657108</v>
       </c>
     </row>
     <row r="226">
@@ -3352,10 +3364,10 @@
         <v>227</v>
       </c>
       <c r="B226" s="1">
-        <v>37.4849508</v>
+        <v>37.5144011</v>
       </c>
       <c r="C226" s="1">
-        <v>126.980963</v>
+        <v>126.8826846</v>
       </c>
     </row>
     <row r="227">
@@ -3363,10 +3375,10 @@
         <v>228</v>
       </c>
       <c r="B227" s="1">
-        <v>37.4844029</v>
+        <v>37.569744</v>
       </c>
       <c r="C227" s="1">
-        <v>126.9716975</v>
+        <v>127.0469446</v>
       </c>
     </row>
     <row r="228">
@@ -3374,10 +3386,10 @@
         <v>229</v>
       </c>
       <c r="B228" s="1">
-        <v>37.4957957</v>
+        <v>37.5586888</v>
       </c>
       <c r="C228" s="1">
-        <v>126.9540341</v>
+        <v>127.0531724</v>
       </c>
     </row>
     <row r="229">
@@ -3385,10 +3397,10 @@
         <v>230</v>
       </c>
       <c r="B229" s="1">
-        <v>37.5028025</v>
+        <v>37.5558896</v>
       </c>
       <c r="C229" s="1">
-        <v>126.9476764</v>
+        <v>126.9556609</v>
       </c>
     </row>
     <row r="230">
@@ -3396,10 +3408,10 @@
         <v>231</v>
       </c>
       <c r="B230" s="1">
-        <v>37.5045422</v>
+        <v>37.5568129</v>
       </c>
       <c r="C230" s="1">
-        <v>126.9385948</v>
+        <v>126.9477118</v>
       </c>
     </row>
     <row r="231">
@@ -3407,10 +3419,10 @@
         <v>232</v>
       </c>
       <c r="B231" s="1">
-        <v>37.4996863</v>
+        <v>37.5178873</v>
       </c>
       <c r="C231" s="1">
-        <v>126.9280893</v>
+        <v>126.8947513</v>
       </c>
     </row>
     <row r="232">
@@ -3418,10 +3430,10 @@
         <v>233</v>
       </c>
       <c r="B232" s="1">
-        <v>37.4998736999999</v>
+        <v>37.4851265</v>
       </c>
       <c r="C232" s="1">
-        <v>126.9205715</v>
+        <v>126.9015288</v>
       </c>
     </row>
     <row r="233">
@@ -3429,10 +3441,10 @@
         <v>234</v>
       </c>
       <c r="B233" s="1">
-        <v>37.5002786</v>
+        <v>37.4875104</v>
       </c>
       <c r="C233" s="1">
-        <v>126.9094236</v>
+        <v>126.9129914</v>
       </c>
     </row>
     <row r="234">
@@ -3440,10 +3452,10 @@
         <v>235</v>
       </c>
       <c r="B234" s="1">
-        <v>37.4860727</v>
+        <v>37.4897586</v>
       </c>
       <c r="C234" s="1">
-        <v>126.8872892</v>
+        <v>126.9230375</v>
       </c>
     </row>
     <row r="235">
@@ -3451,10 +3463,10 @@
         <v>236</v>
       </c>
       <c r="B235" s="1">
-        <v>37.4760554</v>
+        <v>37.4825178</v>
       </c>
       <c r="C235" s="1">
-        <v>126.8679003</v>
+        <v>126.941481</v>
       </c>
     </row>
     <row r="236">
@@ -3462,10 +3474,10 @@
         <v>237</v>
       </c>
       <c r="B236" s="1">
-        <v>37.4792784</v>
+        <v>37.4811133</v>
       </c>
       <c r="C236" s="1">
-        <v>126.8547139</v>
+        <v>126.9526344</v>
       </c>
     </row>
     <row r="237">
@@ -3473,10 +3485,10 @@
         <v>238</v>
       </c>
       <c r="B237" s="1">
-        <v>37.4868662</v>
+        <v>37.4770283</v>
       </c>
       <c r="C237" s="1">
-        <v>126.8388469</v>
+        <v>126.9633959</v>
       </c>
     </row>
     <row r="238">
@@ -3484,10 +3496,10 @@
         <v>239</v>
       </c>
       <c r="B238" s="1">
-        <v>37.5060988</v>
+        <v>37.4812965</v>
       </c>
       <c r="C238" s="1">
-        <v>126.8011495</v>
+        <v>126.9973202</v>
       </c>
     </row>
     <row r="239">
@@ -3495,10 +3507,10 @@
         <v>240</v>
       </c>
       <c r="B239" s="1">
-        <v>37.5050427</v>
+        <v>37.4927648</v>
       </c>
       <c r="C239" s="1">
-        <v>126.7960011</v>
+        <v>127.0105414</v>
       </c>
     </row>
     <row r="240">
@@ -3506,10 +3518,10 @@
         <v>241</v>
       </c>
       <c r="B240" s="1">
-        <v>37.5038999</v>
+        <v>37.4970171999999</v>
       </c>
       <c r="C240" s="1">
-        <v>126.7887438</v>
+        <v>127.0281681</v>
       </c>
     </row>
     <row r="241">
@@ -3517,10 +3529,10 @@
         <v>242</v>
       </c>
       <c r="B241" s="1">
-        <v>37.501902</v>
+        <v>37.4981284</v>
       </c>
       <c r="C241" s="1">
-        <v>126.7762146</v>
+        <v>127.028303</v>
       </c>
     </row>
     <row r="242">
@@ -3528,10 +3540,10 @@
         <v>243</v>
       </c>
       <c r="B242" s="1">
-        <v>37.504159</v>
+        <v>37.5088263</v>
       </c>
       <c r="C242" s="1">
-        <v>126.7672837</v>
+        <v>127.0630673</v>
       </c>
     </row>
     <row r="243">
@@ -3539,10 +3551,10 @@
         <v>244</v>
       </c>
       <c r="B243" s="1">
-        <v>37.5058397</v>
+        <v>37.5115681</v>
       </c>
       <c r="C243" s="1">
-        <v>126.7530584</v>
+        <v>127.0906077</v>
       </c>
     </row>
     <row r="244">
@@ -3550,10 +3562,10 @@
         <v>245</v>
       </c>
       <c r="B244" s="1">
-        <v>37.5068138</v>
+        <v>37.5186216</v>
       </c>
       <c r="C244" s="1">
-        <v>126.7368787</v>
+        <v>127.1049002</v>
       </c>
     </row>
     <row r="245">
@@ -3561,10 +3573,10 @@
         <v>246</v>
       </c>
       <c r="B245" s="1">
-        <v>37.5075879</v>
+        <v>37.5354211</v>
       </c>
       <c r="C245" s="1">
-        <v>126.7208921</v>
+        <v>127.094533</v>
       </c>
     </row>
     <row r="246">
@@ -3572,10 +3584,10 @@
         <v>247</v>
       </c>
       <c r="B246" s="1">
-        <v>37.5511434999999</v>
+        <v>37.5382826</v>
       </c>
       <c r="C246" s="1">
-        <v>127.1281759</v>
+        <v>127.0907553</v>
       </c>
     </row>
     <row r="247">
@@ -3583,10 +3595,10 @@
         <v>248</v>
       </c>
       <c r="B247" s="1">
-        <v>37.5304447</v>
+        <v>37.5446009</v>
       </c>
       <c r="C247" s="1">
-        <v>127.1205399</v>
+        <v>127.0568847</v>
       </c>
     </row>
     <row r="248">
@@ -3594,10 +3606,10 @@
         <v>249</v>
       </c>
       <c r="B248" s="1">
-        <v>37.5169204</v>
+        <v>37.5471773</v>
       </c>
       <c r="C248" s="1">
-        <v>127.1107338</v>
+        <v>127.0473802</v>
       </c>
     </row>
     <row r="249">
@@ -3605,10 +3617,10 @@
         <v>250</v>
       </c>
       <c r="B249" s="1">
-        <v>37.5067662</v>
+        <v>37.5552593</v>
       </c>
       <c r="C249" s="1">
-        <v>127.1054591</v>
+        <v>127.0436579</v>
       </c>
     </row>
     <row r="250">
@@ -3616,10 +3628,10 @@
         <v>251</v>
       </c>
       <c r="B250" s="1">
-        <v>37.4997126</v>
+        <v>37.5639331</v>
       </c>
       <c r="C250" s="1">
-        <v>127.1122396</v>
+        <v>127.0297931</v>
       </c>
     </row>
     <row r="251">
@@ -3627,10 +3639,10 @@
         <v>252</v>
       </c>
       <c r="B251" s="1">
-        <v>37.4881176</v>
+        <v>37.5660664</v>
       </c>
       <c r="C251" s="1">
-        <v>127.1211404</v>
+        <v>126.9820222</v>
       </c>
     </row>
     <row r="252">
@@ -3638,10 +3650,10 @@
         <v>253</v>
       </c>
       <c r="B252" s="1">
-        <v>37.4776196</v>
+        <v>37.565682</v>
       </c>
       <c r="C252" s="1">
-        <v>127.1265061</v>
+        <v>126.9768488</v>
       </c>
     </row>
     <row r="253">
@@ -3649,10 +3661,10 @@
         <v>254</v>
       </c>
       <c r="B253" s="1">
-        <v>37.4706864</v>
+        <v>37.5635313</v>
       </c>
       <c r="C253" s="1">
-        <v>127.1266998</v>
+        <v>126.9755029</v>
       </c>
     </row>
     <row r="254">
@@ -3660,10 +3672,10 @@
         <v>255</v>
       </c>
       <c r="B254" s="1">
-        <v>37.4564664</v>
+        <v>37.5781628</v>
       </c>
       <c r="C254" s="1">
-        <v>127.1500093</v>
+        <v>127.0346872</v>
       </c>
     </row>
     <row r="255">
@@ -3671,10 +3683,10 @@
         <v>256</v>
       </c>
       <c r="B255" s="1">
-        <v>37.4407489</v>
+        <v>37.5708657</v>
       </c>
       <c r="C255" s="1">
-        <v>127.1463494</v>
+        <v>127.0019064</v>
       </c>
     </row>
     <row r="256">
@@ -3682,10 +3694,10 @@
         <v>257</v>
       </c>
       <c r="B256" s="1">
-        <v>37.4374237</v>
+        <v>37.5701747</v>
       </c>
       <c r="C256" s="1">
-        <v>127.1403404</v>
+        <v>126.9832262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code modify and change data
</commit_message>
<xml_diff>
--- a/Second_task/data/address_gps.xlsx
+++ b/Second_task/data/address_gps.xlsx
@@ -12,34 +12,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="C12">
-      <text>
-        <t xml:space="preserve">Geocode : 
-Sorry, no results were found for this address. Please retry by reformulating it or looking for wider results.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C186">
-      <text>
-        <t xml:space="preserve">Geocode : 
-Sorry, no results were found for this address. Please retry by reformulating it or looking for wider results.</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="C220">
-      <text>
-        <t xml:space="preserve">Geocode : 
-Sorry, no results were found for this address. Please retry by reformulating it or looking for wider results.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
   <si>
@@ -829,18 +801,12 @@
     </font>
     <font/>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -849,14 +815,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1009,11 +972,11 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
-        <v>37.539904</v>
-      </c>
-      <c r="C12" s="2">
-        <v>127.017218</v>
+      <c r="B12" s="1">
+        <v>37.5398948</v>
+      </c>
+      <c r="C12" s="1">
+        <v>127.0172208</v>
       </c>
     </row>
     <row r="13">
@@ -2923,11 +2886,11 @@
       <c r="A186" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B186" s="2">
-        <v>37.571747</v>
-      </c>
-      <c r="C186" s="2">
-        <v>127.011172</v>
+      <c r="B186" s="1">
+        <v>37.5717429</v>
+      </c>
+      <c r="C186" s="1">
+        <v>127.0111694</v>
       </c>
     </row>
     <row r="187">
@@ -3297,11 +3260,11 @@
       <c r="A220" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B220" s="2">
-        <v>37.600716</v>
-      </c>
-      <c r="C220" s="2">
-        <v>126.936004</v>
+      <c r="B220" s="1">
+        <v>37.6007016999999</v>
+      </c>
+      <c r="C220" s="1">
+        <v>126.9360048</v>
       </c>
     </row>
     <row r="221">
@@ -3701,7 +3664,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>